<commit_message>
Fixed a bug in AppTimedWrapper.ps1.
</commit_message>
<xml_diff>
--- a/test/results/Benchmarks.xlsx
+++ b/test/results/Benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0516AD56-0A9F-4D85-AF0E-A9829A98537B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C10945-9266-4496-9B25-337F7E850303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -162,35 +162,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -250,13 +232,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -265,13 +240,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -621,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AP75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH65" sqref="AH65"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +740,7 @@
       <c r="C3" s="3">
         <v>833</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="3">
         <v>7153</v>
       </c>
       <c r="E3" s="3">
@@ -790,19 +758,19 @@
       <c r="I3" s="3">
         <v>1786528</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="3">
         <v>2977866</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="3">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="3">
         <v>3</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="3">
         <v>5</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="3">
         <v>204226</v>
       </c>
       <c r="P3" s="1">
@@ -811,7 +779,7 @@
       <c r="Q3" s="3">
         <v>833</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="3">
         <v>7153</v>
       </c>
       <c r="S3" s="3">
@@ -829,29 +797,28 @@
       <c r="W3" s="3">
         <v>1786528</v>
       </c>
-      <c r="X3" s="8">
+      <c r="X3" s="3">
         <v>2977866</v>
       </c>
-      <c r="Y3" s="8">
+      <c r="Y3" s="3">
         <v>2</v>
       </c>
-      <c r="Z3" s="8">
+      <c r="Z3" s="3">
         <v>3</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AA3" s="3">
         <v>5</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AB3" s="3">
         <v>204226</v>
       </c>
-      <c r="AC3" s="5"/>
       <c r="AD3" s="1">
         <v>100</v>
       </c>
       <c r="AE3" s="3">
         <v>833</v>
       </c>
-      <c r="AF3" s="8">
+      <c r="AF3" s="3">
         <v>7153</v>
       </c>
       <c r="AG3" s="3">
@@ -869,19 +836,19 @@
       <c r="AK3" s="3">
         <v>1786528</v>
       </c>
-      <c r="AL3" s="8">
+      <c r="AL3" s="3">
         <v>2977866</v>
       </c>
-      <c r="AM3" s="8">
+      <c r="AM3" s="3">
         <v>2</v>
       </c>
-      <c r="AN3" s="8">
+      <c r="AN3" s="3">
         <v>3</v>
       </c>
-      <c r="AO3" s="8">
+      <c r="AO3" s="3">
         <v>5</v>
       </c>
-      <c r="AP3" s="8">
+      <c r="AP3" s="3">
         <v>204226</v>
       </c>
     </row>
@@ -892,7 +859,7 @@
       <c r="C4" s="3">
         <v>3333</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="3">
         <v>56389</v>
       </c>
       <c r="E4" s="3">
@@ -910,19 +877,19 @@
       <c r="I4" s="3">
         <v>290766028</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="3">
         <v>807151588</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="3">
         <v>2</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="3">
         <v>3</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="3">
         <v>5</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="3">
         <v>190569292</v>
       </c>
       <c r="P4" s="1">
@@ -931,7 +898,7 @@
       <c r="Q4" s="3">
         <v>3333</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="3">
         <v>56389</v>
       </c>
       <c r="S4" s="3">
@@ -949,19 +916,19 @@
       <c r="W4" s="3">
         <v>290766028</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X4" s="3">
         <v>807151588</v>
       </c>
-      <c r="Y4" s="8">
+      <c r="Y4" s="3">
         <v>2</v>
       </c>
-      <c r="Z4" s="8">
+      <c r="Z4" s="3">
         <v>3</v>
       </c>
-      <c r="AA4" s="8">
+      <c r="AA4" s="3">
         <v>5</v>
       </c>
-      <c r="AB4" s="8">
+      <c r="AB4" s="3">
         <v>190569292</v>
       </c>
       <c r="AD4" s="1">
@@ -970,7 +937,7 @@
       <c r="AE4" s="3">
         <v>3333</v>
       </c>
-      <c r="AF4" s="8">
+      <c r="AF4" s="3">
         <v>56389</v>
       </c>
       <c r="AG4" s="3">
@@ -988,19 +955,19 @@
       <c r="AK4" s="3">
         <v>290766028</v>
       </c>
-      <c r="AL4" s="8">
+      <c r="AL4" s="3">
         <v>807151588</v>
       </c>
-      <c r="AM4" s="8">
+      <c r="AM4" s="3">
         <v>2</v>
       </c>
-      <c r="AN4" s="8">
+      <c r="AN4" s="3">
         <v>3</v>
       </c>
-      <c r="AO4" s="8">
+      <c r="AO4" s="3">
         <v>5</v>
       </c>
-      <c r="AP4" s="8">
+      <c r="AP4" s="3">
         <v>190569292</v>
       </c>
     </row>
@@ -1011,7 +978,7 @@
       <c r="C5" s="3">
         <v>7500</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="3">
         <v>189375</v>
       </c>
       <c r="E5" s="3">
@@ -1023,25 +990,25 @@
       <c r="G5" s="3">
         <v>230282157</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="3">
         <v>1348858067</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="3">
         <v>6333941094</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="3">
         <v>24613920986</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="3">
         <v>2</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="3">
         <v>3</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="3">
         <v>5</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="3">
         <v>40853235313</v>
       </c>
       <c r="P5" s="1">
@@ -1050,7 +1017,7 @@
       <c r="Q5" s="3">
         <v>7500</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="3">
         <v>189375</v>
       </c>
       <c r="S5" s="3">
@@ -1062,35 +1029,34 @@
       <c r="U5" s="3">
         <v>230282157</v>
       </c>
-      <c r="V5" s="8">
+      <c r="V5" s="3">
         <v>1348858067</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="3">
         <v>6333941094</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="3">
         <v>24613920986</v>
       </c>
-      <c r="Y5" s="8">
+      <c r="Y5" s="3">
         <v>2</v>
       </c>
-      <c r="Z5" s="8">
+      <c r="Z5" s="3">
         <v>3</v>
       </c>
-      <c r="AA5" s="8">
+      <c r="AA5" s="3">
         <v>5</v>
       </c>
-      <c r="AB5" s="8">
+      <c r="AB5" s="3">
         <v>40853235313</v>
       </c>
-      <c r="AC5" s="5"/>
       <c r="AD5" s="1">
         <v>300</v>
       </c>
       <c r="AE5" s="3">
         <v>7500</v>
       </c>
-      <c r="AF5" s="8">
+      <c r="AF5" s="3">
         <v>189375</v>
       </c>
       <c r="AG5" s="3">
@@ -1102,25 +1068,25 @@
       <c r="AI5" s="3">
         <v>230282157</v>
       </c>
-      <c r="AJ5" s="8">
+      <c r="AJ5" s="3">
         <v>1348858067</v>
       </c>
-      <c r="AK5" s="8">
+      <c r="AK5" s="3">
         <v>6333941094</v>
       </c>
-      <c r="AL5" s="8">
+      <c r="AL5" s="3">
         <v>24613920986</v>
       </c>
-      <c r="AM5" s="8">
+      <c r="AM5" s="3">
         <v>2</v>
       </c>
-      <c r="AN5" s="8">
+      <c r="AN5" s="3">
         <v>3</v>
       </c>
-      <c r="AO5" s="8">
+      <c r="AO5" s="3">
         <v>5</v>
       </c>
-      <c r="AP5" s="8">
+      <c r="AP5" s="3">
         <v>40853235313</v>
       </c>
     </row>
@@ -1131,7 +1097,7 @@
       <c r="C6" s="3">
         <v>13333</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="3">
         <v>447778</v>
       </c>
       <c r="E6" s="3">
@@ -1143,25 +1109,25 @@
       <c r="G6" s="3">
         <v>1251251004</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="3">
         <v>9563419823</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="3">
         <v>58187547820</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="3">
         <v>290737409717</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="3">
         <v>2</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="3">
         <v>3</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="3">
         <v>5</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="3">
         <v>3972999029388</v>
       </c>
       <c r="P6" s="1">
@@ -1170,7 +1136,7 @@
       <c r="Q6" s="3">
         <v>13333</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="3">
         <v>447778</v>
       </c>
       <c r="S6" s="3">
@@ -1182,35 +1148,34 @@
       <c r="U6" s="3">
         <v>1251251004</v>
       </c>
-      <c r="V6" s="8">
+      <c r="V6" s="3">
         <v>9563419823</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W6" s="3">
         <v>58187547820</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X6" s="3">
         <v>290737409717</v>
       </c>
-      <c r="Y6" s="8">
+      <c r="Y6" s="3">
         <v>2</v>
       </c>
-      <c r="Z6" s="8">
+      <c r="Z6" s="3">
         <v>3</v>
       </c>
-      <c r="AA6" s="8">
+      <c r="AA6" s="3">
         <v>5</v>
       </c>
-      <c r="AB6" s="8">
+      <c r="AB6" s="3">
         <v>3972999029388</v>
       </c>
-      <c r="AC6" s="5"/>
       <c r="AD6" s="1">
         <v>400</v>
       </c>
       <c r="AE6" s="3">
         <v>13333</v>
       </c>
-      <c r="AF6" s="8">
+      <c r="AF6" s="3">
         <v>447778</v>
       </c>
       <c r="AG6" s="3">
@@ -1222,25 +1187,25 @@
       <c r="AI6" s="3">
         <v>1251251004</v>
       </c>
-      <c r="AJ6" s="8">
+      <c r="AJ6" s="3">
         <v>9563419823</v>
       </c>
-      <c r="AK6" s="8">
+      <c r="AK6" s="3">
         <v>58187547820</v>
       </c>
-      <c r="AL6" s="8">
+      <c r="AL6" s="3">
         <v>290737409717</v>
       </c>
-      <c r="AM6" s="8">
+      <c r="AM6" s="3">
         <v>2</v>
       </c>
-      <c r="AN6" s="8">
+      <c r="AN6" s="3">
         <v>3</v>
       </c>
-      <c r="AO6" s="8">
+      <c r="AO6" s="3">
         <v>5</v>
       </c>
-      <c r="AP6" s="8">
+      <c r="AP6" s="3">
         <v>3972999029388</v>
       </c>
     </row>
@@ -1263,25 +1228,25 @@
       <c r="G7" s="3">
         <v>4677232746</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="3">
         <v>44100541271</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="3">
         <v>329567334191</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="3">
         <v>2012762670309</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="3">
         <v>2</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="3">
         <v>3</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="3">
         <v>5</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="3">
         <v>230793554364681</v>
       </c>
       <c r="P7" s="1">
@@ -1302,28 +1267,27 @@
       <c r="U7" s="3">
         <v>4677232746</v>
       </c>
-      <c r="V7" s="8">
+      <c r="V7" s="3">
         <v>44100541271</v>
       </c>
-      <c r="W7" s="8">
+      <c r="W7" s="3">
         <v>329567334191</v>
       </c>
-      <c r="X7" s="8">
+      <c r="X7" s="3">
         <v>2012762670309</v>
       </c>
-      <c r="Y7" s="8">
+      <c r="Y7" s="3">
         <v>2</v>
       </c>
-      <c r="Z7" s="8">
+      <c r="Z7" s="3">
         <v>3</v>
       </c>
-      <c r="AA7" s="8">
+      <c r="AA7" s="3">
         <v>5</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AB7" s="3">
         <v>230793554364681</v>
       </c>
-      <c r="AC7" s="5"/>
       <c r="AD7" s="1">
         <v>500</v>
       </c>
@@ -1342,25 +1306,25 @@
       <c r="AI7" s="3">
         <v>4677232746</v>
       </c>
-      <c r="AJ7" s="8">
+      <c r="AJ7" s="3">
         <v>44100541271</v>
       </c>
-      <c r="AK7" s="8">
+      <c r="AK7" s="3">
         <v>329567334191</v>
       </c>
-      <c r="AL7" s="8">
+      <c r="AL7" s="3">
         <v>2012762670309</v>
       </c>
-      <c r="AM7" s="8">
+      <c r="AM7" s="3">
         <v>2</v>
       </c>
-      <c r="AN7" s="8">
+      <c r="AN7" s="3">
         <v>3</v>
       </c>
-      <c r="AO7" s="8">
+      <c r="AO7" s="3">
         <v>5</v>
       </c>
-      <c r="AP7" s="8">
+      <c r="AP7" s="3">
         <v>230793554364681</v>
       </c>
     </row>
@@ -1443,7 +1407,6 @@
       <c r="AB8" s="3">
         <v>9253082936723600</v>
       </c>
-      <c r="AC8" s="5"/>
       <c r="AD8" s="1">
         <v>600</v>
       </c>
@@ -1524,7 +1487,6 @@
       <c r="N9" s="3">
         <v>2.7936332848370202E+17</v>
       </c>
-      <c r="O9" s="7"/>
       <c r="P9" s="1">
         <v>700</v>
       </c>
@@ -1564,7 +1526,6 @@
       <c r="AB9" s="3">
         <v>2.7936332848370202E+17</v>
       </c>
-      <c r="AC9" s="5"/>
       <c r="AD9" s="1">
         <v>700</v>
       </c>
@@ -1645,7 +1606,6 @@
       <c r="N10" s="3">
         <v>6.7270900517410396E+18</v>
       </c>
-      <c r="O10" s="7"/>
       <c r="P10" s="1">
         <v>800</v>
       </c>
@@ -1685,7 +1645,6 @@
       <c r="AB10" s="3">
         <v>6.7270900517410396E+18</v>
       </c>
-      <c r="AC10" s="5"/>
       <c r="AD10" s="1">
         <v>800</v>
       </c>
@@ -1766,7 +1725,6 @@
       <c r="N11" s="3">
         <v>1.34508188001572E+20</v>
       </c>
-      <c r="O11" s="7"/>
       <c r="P11" s="1">
         <v>900</v>
       </c>
@@ -1806,7 +1764,6 @@
       <c r="AB11" s="3">
         <v>1.34508188001572E+20</v>
       </c>
-      <c r="AC11" s="5"/>
       <c r="AD11" s="1">
         <v>900</v>
       </c>
@@ -1887,7 +1844,6 @@
       <c r="N12" s="3">
         <v>2.3001650325743201E+21</v>
       </c>
-      <c r="O12" s="7"/>
       <c r="P12" s="1">
         <v>1000</v>
       </c>
@@ -1927,7 +1883,6 @@
       <c r="AB12" s="3">
         <v>2.3001650325743201E+21</v>
       </c>
-      <c r="AC12" s="5"/>
       <c r="AD12" s="1">
         <v>1000</v>
       </c>
@@ -2008,7 +1963,6 @@
       <c r="N13" s="3">
         <v>3.4403115367205001E+22</v>
       </c>
-      <c r="O13" s="7"/>
       <c r="P13" s="1">
         <v>1100</v>
       </c>
@@ -2048,7 +2002,6 @@
       <c r="AB13" s="3">
         <v>3.4403115367205001E+22</v>
       </c>
-      <c r="AC13" s="5"/>
       <c r="AD13" s="1">
         <v>1100</v>
       </c>
@@ -2129,7 +2082,6 @@
       <c r="N14" s="3">
         <v>4.5800478800814402E+23</v>
       </c>
-      <c r="O14" s="7"/>
       <c r="P14" s="1">
         <v>1200</v>
       </c>
@@ -2169,7 +2121,6 @@
       <c r="AB14" s="3">
         <v>4.5800478800814402E+23</v>
       </c>
-      <c r="AC14" s="5"/>
       <c r="AD14" s="1">
         <v>1200</v>
       </c>
@@ -2250,7 +2201,6 @@
       <c r="N15" s="3">
         <v>5.5036377624997203E+24</v>
       </c>
-      <c r="O15" s="7"/>
       <c r="P15" s="1">
         <v>1300</v>
       </c>
@@ -2370,7 +2320,6 @@
       <c r="N16" s="3">
         <v>6.0378285202834401E+25</v>
       </c>
-      <c r="O16" s="7"/>
       <c r="P16" s="1">
         <v>1400</v>
       </c>
@@ -2490,7 +2439,6 @@
       <c r="N17" s="3">
         <v>6.1045074711796603E+26</v>
       </c>
-      <c r="O17" s="7"/>
       <c r="P17" s="1">
         <v>1500</v>
       </c>
@@ -2610,7 +2558,6 @@
       <c r="N18" s="3">
         <v>2.4061467864032602E+31</v>
       </c>
-      <c r="O18" s="7"/>
       <c r="P18" s="1">
         <v>2000</v>
       </c>
@@ -2730,7 +2677,6 @@
       <c r="N19" s="3">
         <v>1.32946169076319E+39</v>
       </c>
-      <c r="O19" s="7"/>
       <c r="P19" s="1">
         <v>3000</v>
       </c>
@@ -2850,7 +2796,6 @@
       <c r="N20" s="3">
         <v>4.72081917561941E+45</v>
       </c>
-      <c r="O20" s="7"/>
       <c r="P20" s="1">
         <v>4000</v>
       </c>
@@ -2970,7 +2915,6 @@
       <c r="N21" s="3">
         <v>2.8708755106413501E+51</v>
       </c>
-      <c r="O21" s="7"/>
       <c r="P21" s="1">
         <v>5000</v>
       </c>
@@ -3090,7 +3034,6 @@
       <c r="N22" s="3">
         <v>1.6982016882544199E+74</v>
       </c>
-      <c r="O22" s="7"/>
       <c r="P22" s="1">
         <v>10000</v>
       </c>
@@ -3208,7 +3151,6 @@
         <v>5</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="7"/>
       <c r="P23" s="1">
         <v>20000</v>
       </c>
@@ -3322,7 +3264,6 @@
         <v>5</v>
       </c>
       <c r="N24" s="4"/>
-      <c r="O24" s="7"/>
       <c r="P24" s="1">
         <v>30000</v>
       </c>
@@ -3436,7 +3377,6 @@
         <v>5</v>
       </c>
       <c r="N25" s="4"/>
-      <c r="O25" s="7"/>
       <c r="P25" s="1">
         <v>40000</v>
       </c>
@@ -6749,7 +6689,7 @@
         <v>200</v>
       </c>
       <c r="AE54" s="2">
-        <f t="shared" ref="AE54:AP54" si="5">AE4/AE29</f>
+        <f t="shared" ref="AE54:AO54" si="5">AE4/AE29</f>
         <v>0.21017782822550132</v>
       </c>
       <c r="AF54" s="2">
@@ -6898,7 +6838,7 @@
         <v>300</v>
       </c>
       <c r="AE55" s="2">
-        <f t="shared" ref="AE55:AP55" si="8">AE5/AE30</f>
+        <f t="shared" ref="AE55:AO55" si="8">AE5/AE30</f>
         <v>0.24079365588981283</v>
       </c>
       <c r="AF55" s="2">
@@ -6946,7 +6886,7 @@
         <v>400</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" ref="C56:N56" si="9">C6/C31</f>
+        <f t="shared" ref="C56:M56" si="9">C6/C31</f>
         <v>98.762962962962959</v>
       </c>
       <c r="D56" s="2">
@@ -6995,7 +6935,7 @@
         <v>400</v>
       </c>
       <c r="Q56" s="2">
-        <f t="shared" ref="Q56:AB56" si="10">Q6/Q31</f>
+        <f t="shared" ref="Q56:AA56" si="10">Q6/Q31</f>
         <v>1.173886247578799</v>
       </c>
       <c r="R56" s="2">
@@ -7042,7 +6982,7 @@
         <v>400</v>
       </c>
       <c r="AE56" s="2">
-        <f t="shared" ref="AE56:AP56" si="11">AE6/AE31</f>
+        <f t="shared" ref="AE56:AO56" si="11">AE6/AE31</f>
         <v>0.25090799601046315</v>
       </c>
       <c r="AF56" s="2">
@@ -7089,7 +7029,7 @@
         <v>500</v>
       </c>
       <c r="C57" s="2">
-        <f t="shared" ref="C57:N57" si="12">C7/C32</f>
+        <f t="shared" ref="C57:M57" si="12">C7/C32</f>
         <v>87.1673640167364</v>
       </c>
       <c r="D57" s="2">
@@ -7137,7 +7077,7 @@
         <v>500</v>
       </c>
       <c r="Q57" s="2">
-        <f t="shared" ref="Q57:AB57" si="13">Q7/Q32</f>
+        <f t="shared" ref="Q57:AA57" si="13">Q7/Q32</f>
         <v>0.94587968217934171</v>
       </c>
       <c r="R57" s="2">
@@ -7183,7 +7123,7 @@
         <v>500</v>
       </c>
       <c r="AE57" s="2">
-        <f t="shared" ref="AE57:AP57" si="14">AE7/AE32</f>
+        <f t="shared" ref="AE57:AO57" si="14">AE7/AE32</f>
         <v>0.25728646939682853</v>
       </c>
       <c r="AF57" s="2">
@@ -7230,7 +7170,7 @@
         <v>600</v>
       </c>
       <c r="C58" s="2">
-        <f t="shared" ref="C58:N58" si="15">C8/C33</f>
+        <f t="shared" ref="C58:M58" si="15">C8/C33</f>
         <v>101.35135135135135</v>
       </c>
       <c r="D58" s="2">
@@ -7277,7 +7217,7 @@
         <v>600</v>
       </c>
       <c r="Q58" s="2">
-        <f t="shared" ref="Q58:AB58" si="16">Q8/Q33</f>
+        <f t="shared" ref="Q58:AA58" si="16">Q8/Q33</f>
         <v>0.99555319572575829</v>
       </c>
       <c r="R58" s="2">
@@ -7323,7 +7263,7 @@
         <v>600</v>
       </c>
       <c r="AE58" s="2">
-        <f t="shared" ref="AE58:AP58" si="17">AE8/AE33</f>
+        <f t="shared" ref="AE58:AO58" si="17">AE8/AE33</f>
         <v>0.23210292991265194</v>
       </c>
       <c r="AF58" s="2">
@@ -7370,7 +7310,7 @@
         <v>700</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" ref="C59:N59" si="18">C9/C34</f>
+        <f t="shared" ref="C59:M59" si="18">C9/C34</f>
         <v>56.166437414030263</v>
       </c>
       <c r="D59" s="2">
@@ -7417,7 +7357,7 @@
         <v>700</v>
       </c>
       <c r="Q59" s="2">
-        <f t="shared" ref="Q59:AB59" si="19">Q9/Q34</f>
+        <f t="shared" ref="Q59:AA59" si="19">Q9/Q34</f>
         <v>0.86185571362235636</v>
       </c>
       <c r="R59" s="2">
@@ -7462,7 +7402,7 @@
         <v>700</v>
       </c>
       <c r="AE59" s="2">
-        <f t="shared" ref="AE59:AP59" si="20">AE9/AE34</f>
+        <f t="shared" ref="AE59:AO59" si="20">AE9/AE34</f>
         <v>0.21975319272602026</v>
       </c>
       <c r="AF59" s="2">
@@ -7508,7 +7448,7 @@
         <v>800</v>
       </c>
       <c r="C60" s="2">
-        <f t="shared" ref="C60:N60" si="21">C10/C35</f>
+        <f t="shared" ref="C60:M60" si="21">C10/C35</f>
         <v>136.75128205128206</v>
       </c>
       <c r="D60" s="2">
@@ -7554,7 +7494,7 @@
         <v>800</v>
       </c>
       <c r="Q60" s="2">
-        <f t="shared" ref="Q60:AB60" si="22">Q10/Q35</f>
+        <f t="shared" ref="Q60:AA60" si="22">Q10/Q35</f>
         <v>0.87250924320256518</v>
       </c>
       <c r="R60" s="2">
@@ -7599,7 +7539,7 @@
         <v>800</v>
       </c>
       <c r="AE60" s="2">
-        <f t="shared" ref="AE60:AP60" si="23">AE10/AE35</f>
+        <f t="shared" ref="AE60:AO60" si="23">AE10/AE35</f>
         <v>0.17670934223953985</v>
       </c>
       <c r="AF60" s="2">
@@ -7645,7 +7585,7 @@
         <v>900</v>
       </c>
       <c r="C61" s="2">
-        <f t="shared" ref="C61:N61" si="24">C11/C36</f>
+        <f t="shared" ref="C61:M61" si="24">C11/C36</f>
         <v>66.633761105626846</v>
       </c>
       <c r="D61" s="2">
@@ -7691,7 +7631,7 @@
         <v>900</v>
       </c>
       <c r="Q61" s="2">
-        <f t="shared" ref="Q61:AB61" si="25">Q11/Q36</f>
+        <f t="shared" ref="Q61:AA61" si="25">Q11/Q36</f>
         <v>0.79738222369229317</v>
       </c>
       <c r="R61" s="2">
@@ -7736,7 +7676,7 @@
         <v>900</v>
       </c>
       <c r="AE61" s="2">
-        <f t="shared" ref="AE61:AP61" si="26">AE11/AE36</f>
+        <f t="shared" ref="AE61:AO61" si="26">AE11/AE36</f>
         <v>0.18223837319179037</v>
       </c>
       <c r="AF61" s="2">
@@ -7782,7 +7722,7 @@
         <v>1000</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" ref="C62:N62" si="27">C12/C37</f>
+        <f t="shared" ref="C62:M62" si="27">C12/C37</f>
         <v>97.011641443539006</v>
       </c>
       <c r="D62" s="2">
@@ -7828,7 +7768,7 @@
         <v>1000</v>
       </c>
       <c r="Q62" s="2">
-        <f t="shared" ref="Q62:AB62" si="28">Q12/Q37</f>
+        <f t="shared" ref="Q62:AA62" si="28">Q12/Q37</f>
         <v>0.7604833042827549</v>
       </c>
       <c r="R62" s="2">
@@ -7872,7 +7812,7 @@
         <v>1000</v>
       </c>
       <c r="AE62" s="2">
-        <f t="shared" ref="AE62:AP62" si="29">AE12/AE37</f>
+        <f t="shared" ref="AE62:AO62" si="29">AE12/AE37</f>
         <v>0.18117011724652207</v>
       </c>
       <c r="AF62" s="2">
@@ -7918,7 +7858,7 @@
         <v>1100</v>
       </c>
       <c r="C63" s="2">
-        <f t="shared" ref="C63:N63" si="30">C13/C38</f>
+        <f t="shared" ref="C63:M63" si="30">C13/C38</f>
         <v>80.34501992031872</v>
       </c>
       <c r="D63" s="2">
@@ -7964,7 +7904,7 @@
         <v>1100</v>
       </c>
       <c r="Q63" s="2">
-        <f t="shared" ref="Q63:AB63" si="31">Q13/Q38</f>
+        <f t="shared" ref="Q63:AA63" si="31">Q13/Q38</f>
         <v>0.60333159812597603</v>
       </c>
       <c r="R63" s="2">
@@ -8008,7 +7948,7 @@
         <v>1100</v>
       </c>
       <c r="AE63" s="2">
-        <f t="shared" ref="AE63:AP63" si="32">AE13/AE38</f>
+        <f t="shared" ref="AE63:AO63" si="32">AE13/AE38</f>
         <v>0.17078904801023043</v>
       </c>
       <c r="AF63" s="2">
@@ -8054,7 +7994,7 @@
         <v>1200</v>
       </c>
       <c r="C64" s="2">
-        <f t="shared" ref="C64:N64" si="33">C14/C39</f>
+        <f t="shared" ref="C64:M64" si="33">C14/C39</f>
         <v>122.69938650306749</v>
       </c>
       <c r="D64" s="2">
@@ -8100,7 +8040,7 @@
         <v>1200</v>
       </c>
       <c r="Q64" s="2">
-        <f t="shared" ref="Q64:AB64" si="34">Q14/Q39</f>
+        <f t="shared" ref="Q64:AA64" si="34">Q14/Q39</f>
         <v>0.58507474329845632</v>
       </c>
       <c r="R64" s="2">
@@ -8144,7 +8084,7 @@
         <v>1200</v>
       </c>
       <c r="AE64" s="2">
-        <f t="shared" ref="AE64:AP64" si="35">AE14/AE39</f>
+        <f t="shared" ref="AE64:AO64" si="35">AE14/AE39</f>
         <v>0.1654809496951703</v>
       </c>
       <c r="AF64" s="2">
@@ -8190,7 +8130,7 @@
         <v>1300</v>
       </c>
       <c r="C65" s="2">
-        <f t="shared" ref="C65:N65" si="36">C15/C40</f>
+        <f t="shared" ref="C65:M65" si="36">C15/C40</f>
         <v>84.23026315789474</v>
       </c>
       <c r="D65" s="2">
@@ -8236,7 +8176,7 @@
         <v>1300</v>
       </c>
       <c r="Q65" s="2">
-        <f t="shared" ref="Q65:AB65" si="37">Q15/Q40</f>
+        <f t="shared" ref="Q65:AA65" si="37">Q15/Q40</f>
         <v>0.55199187884108869</v>
       </c>
       <c r="R65" s="2">
@@ -8280,7 +8220,7 @@
         <v>1300</v>
       </c>
       <c r="AE65" s="2">
-        <f t="shared" ref="AE65:AP65" si="38">AE15/AE40</f>
+        <f t="shared" ref="AE65:AO65" si="38">AE15/AE40</f>
         <v>0.15370301451432825</v>
       </c>
       <c r="AF65" s="2">
@@ -8326,7 +8266,7 @@
         <v>1400</v>
       </c>
       <c r="C66" s="2">
-        <f t="shared" ref="C66:N66" si="39">C16/C41</f>
+        <f t="shared" ref="C66:M66" si="39">C16/C41</f>
         <v>104.56658130601792</v>
       </c>
       <c r="D66" s="2">
@@ -8372,7 +8312,7 @@
         <v>1400</v>
       </c>
       <c r="Q66" s="2">
-        <f t="shared" ref="Q66:AB66" si="40">Q16/Q41</f>
+        <f t="shared" ref="Q66:AA66" si="40">Q16/Q41</f>
         <v>0.52588147036759192</v>
       </c>
       <c r="R66" s="2">
@@ -8416,7 +8356,7 @@
         <v>1400</v>
       </c>
       <c r="AE66" s="2">
-        <f t="shared" ref="AE66:AP66" si="41">AE16/AE41</f>
+        <f t="shared" ref="AE66:AO66" si="41">AE16/AE41</f>
         <v>0.13812644345951633</v>
       </c>
       <c r="AF66" s="2">
@@ -8462,7 +8402,7 @@
         <v>1500</v>
       </c>
       <c r="C67" s="2">
-        <f t="shared" ref="C67:N67" si="42">C17/C42</f>
+        <f t="shared" ref="C67:M67" si="42">C17/C42</f>
         <v>114.39902379499695</v>
       </c>
       <c r="D67" s="2">
@@ -8507,7 +8447,7 @@
         <v>1500</v>
       </c>
       <c r="Q67" s="2">
-        <f t="shared" ref="Q67:AB67" si="43">Q17/Q42</f>
+        <f t="shared" ref="Q67:AA67" si="43">Q17/Q42</f>
         <v>0.25303712020815172</v>
       </c>
       <c r="R67" s="2">
@@ -8551,7 +8491,7 @@
         <v>1500</v>
       </c>
       <c r="AE67" s="2">
-        <f t="shared" ref="AE67:AP67" si="44">AE17/AE42</f>
+        <f t="shared" ref="AE67:AO67" si="44">AE17/AE42</f>
         <v>7.3632410513058855E-2</v>
       </c>
       <c r="AF67" s="2" t="s">
@@ -8596,7 +8536,7 @@
         <v>2000</v>
       </c>
       <c r="C68" s="2">
-        <f t="shared" ref="C68:N68" si="45">C18/C43</f>
+        <f t="shared" ref="C68:M68" si="45">C18/C43</f>
         <v>104.1665625</v>
       </c>
       <c r="D68" s="2">
@@ -8641,7 +8581,7 @@
         <v>2000</v>
       </c>
       <c r="Q68" s="2">
-        <f t="shared" ref="Q68:AB68" si="46">Q18/Q43</f>
+        <f t="shared" ref="Q68:AA68" si="46">Q18/Q43</f>
         <v>0.12705568360663674</v>
       </c>
       <c r="R68" s="2">
@@ -8685,7 +8625,7 @@
         <v>2000</v>
       </c>
       <c r="AE68" s="2">
-        <f t="shared" ref="AE68:AP68" si="47">AE18/AE43</f>
+        <f t="shared" ref="AE68:AO68" si="47">AE18/AE43</f>
         <v>3.864313760950993E-2</v>
       </c>
       <c r="AF68" s="2" t="s">
@@ -8730,7 +8670,7 @@
         <v>3000</v>
       </c>
       <c r="C69" s="2">
-        <f t="shared" ref="C69:N69" si="48">C19/C44</f>
+        <f t="shared" ref="C69:M69" si="48">C19/C44</f>
         <v>80.454838017592792</v>
       </c>
       <c r="D69" s="2">
@@ -8775,7 +8715,7 @@
         <v>3000</v>
       </c>
       <c r="Q69" s="2">
-        <f t="shared" ref="Q69:AB69" si="49">Q19/Q44</f>
+        <f t="shared" ref="Q69:AA69" si="49">Q19/Q44</f>
         <v>0.11742065338487735</v>
       </c>
       <c r="R69" s="2">
@@ -8819,7 +8759,7 @@
         <v>3000</v>
       </c>
       <c r="AE69" s="2">
-        <f t="shared" ref="AE69:AP69" si="50">AE19/AE44</f>
+        <f t="shared" ref="AE69:AO69" si="50">AE19/AE44</f>
         <v>3.7762582114734808E-2</v>
       </c>
       <c r="AF69" s="2" t="s">
@@ -8864,7 +8804,7 @@
         <v>4000</v>
       </c>
       <c r="C70" s="2">
-        <f t="shared" ref="C70:N70" si="51">C20/C45</f>
+        <f t="shared" ref="C70:M70" si="51">C20/C45</f>
         <v>72.526816797214963</v>
       </c>
       <c r="D70" s="2">
@@ -8908,7 +8848,7 @@
         <v>4000</v>
       </c>
       <c r="Q70" s="2">
-        <f t="shared" ref="Q70:AB70" si="52">Q20/Q45</f>
+        <f t="shared" ref="Q70:AA70" si="52">Q20/Q45</f>
         <v>0.10101217252539939</v>
       </c>
       <c r="R70" s="2" t="s">
@@ -8951,7 +8891,7 @@
         <v>4000</v>
       </c>
       <c r="AE70" s="2">
-        <f t="shared" ref="AE70:AP70" si="53">AE20/AE45</f>
+        <f t="shared" ref="AE70:AO70" si="53">AE20/AE45</f>
         <v>3.4780273955765273E-2</v>
       </c>
       <c r="AF70" s="2" t="s">
@@ -8996,7 +8936,7 @@
         <v>5000</v>
       </c>
       <c r="C71" s="2">
-        <f t="shared" ref="C71:N71" si="54">C21/C46</f>
+        <f t="shared" ref="C71:M71" si="54">C21/C46</f>
         <v>59.649916967302296</v>
       </c>
       <c r="D71" s="2">
@@ -9040,7 +8980,7 @@
         <v>5000</v>
       </c>
       <c r="Q71" s="2">
-        <f t="shared" ref="Q71:AB71" si="55">Q21/Q46</f>
+        <f t="shared" ref="Q71:AA71" si="55">Q21/Q46</f>
         <v>1.9361745742511746E-2</v>
       </c>
       <c r="R71" s="2" t="s">
@@ -9083,7 +9023,7 @@
         <v>5000</v>
       </c>
       <c r="AE71" s="2">
-        <f t="shared" ref="AE71:AP71" si="56">AE21/AE46</f>
+        <f t="shared" ref="AE71:AO71" si="56">AE21/AE46</f>
         <v>6.8901970872731156E-3</v>
       </c>
       <c r="AF71" s="2" t="s">
@@ -9128,7 +9068,7 @@
         <v>10000</v>
       </c>
       <c r="C72" s="2">
-        <f t="shared" ref="C72:N72" si="57">C22/C47</f>
+        <f t="shared" ref="C72:M72" si="57">C22/C47</f>
         <v>72.641262563306867</v>
       </c>
       <c r="D72" s="2">
@@ -9196,7 +9136,7 @@
         <v>1</v>
       </c>
       <c r="Y72" s="2">
-        <f t="shared" ref="Q72:AB72" si="58">Y22/Y47</f>
+        <f t="shared" ref="Y72:AA72" si="58">Y22/Y47</f>
         <v>2</v>
       </c>
       <c r="Z72" s="2">
@@ -9255,7 +9195,7 @@
         <v>20000</v>
       </c>
       <c r="C73" s="2">
-        <f t="shared" ref="C73:N73" si="59">C23/C48</f>
+        <f t="shared" ref="C73:M73" si="59">C23/C48</f>
         <v>70.985418884961035</v>
       </c>
       <c r="D73" s="2">
@@ -9323,7 +9263,7 @@
         <v>1</v>
       </c>
       <c r="Y73" s="2">
-        <f t="shared" ref="Q73:AB73" si="60">Y23/Y48</f>
+        <f t="shared" ref="Y73:AA73" si="60">Y23/Y48</f>
         <v>2</v>
       </c>
       <c r="Z73" s="2">
@@ -9382,7 +9322,7 @@
         <v>30000</v>
       </c>
       <c r="C74" s="2">
-        <f t="shared" ref="C74:N74" si="61">C24/C49</f>
+        <f t="shared" ref="C74:M74" si="61">C24/C49</f>
         <v>71.930578360212991</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -9449,7 +9389,7 @@
         <v>1</v>
       </c>
       <c r="Y74" s="2">
-        <f t="shared" ref="Q74:AB74" si="62">Y24/Y49</f>
+        <f t="shared" ref="Y74:AA74" si="62">Y24/Y49</f>
         <v>2</v>
       </c>
       <c r="Z74" s="2">
@@ -9532,7 +9472,7 @@
         <v>1</v>
       </c>
       <c r="K75" s="2">
-        <f t="shared" ref="C75:N75" si="63">K25/K50</f>
+        <f t="shared" ref="K75:M75" si="63">K25/K50</f>
         <v>7.9365079365079361E-3</v>
       </c>
       <c r="L75" s="2">
@@ -9574,7 +9514,7 @@
         <v>1</v>
       </c>
       <c r="Y75" s="2">
-        <f t="shared" ref="Q75:AB75" si="64">Y25/Y50</f>
+        <f t="shared" ref="Y75:AA75" si="64">Y25/Y50</f>
         <v>2</v>
       </c>
       <c r="Z75" s="2">
@@ -9629,19 +9569,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 AT2:XFD55 B27:AS51 A76:XFD1048576 B2:N2 B3:B25 C25:N25 P2:AB2 P3:P25 Q25:AB25 A2:A75 AQ56:XFD75 AQ52:AS55 B52:AP75">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 B2:N2 P2:AB2 AT2:XFD55 A2:A75 B3:B25 P3:P25 C25:N25 Q25:AB25 B27:AS51 AQ52:AS55 B52:AP75 AQ56:XFD75 A76:XFD1048576">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AP2 AD3:AD25 AE25:AP25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9652,7 +9592,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
-  <dimension ref="B2:AK66"/>
+  <dimension ref="B2:AF42"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M35" sqref="M35"/>
@@ -12168,7 +12108,7 @@
         <v>0.75877721167207035</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" ref="T31:AF31" si="1">T3/T17</f>
+        <f t="shared" ref="T31:AE31" si="1">T3/T17</f>
         <v>1.1644237624920624</v>
       </c>
       <c r="U31" s="3" t="s">
@@ -12260,7 +12200,7 @@
         <v>16</v>
       </c>
       <c r="S32" s="3">
-        <f t="shared" ref="S32:AF32" si="3">S4/S18</f>
+        <f t="shared" ref="S32:AE32" si="3">S4/S18</f>
         <v>0.68527271206290785</v>
       </c>
       <c r="T32" s="3" t="s">
@@ -12302,12 +12242,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>18</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" ref="C33:P33" si="4">C5/C19</f>
+        <f t="shared" ref="C33:O33" si="4">C5/C19</f>
         <v>169.78108808290156</v>
       </c>
       <c r="D33" s="3">
@@ -12357,7 +12297,7 @@
         <v>18</v>
       </c>
       <c r="S33" s="3">
-        <f t="shared" ref="S33:AF33" si="5">S5/S19</f>
+        <f t="shared" ref="S33:AE33" si="5">S5/S19</f>
         <v>1.0261085363562348</v>
       </c>
       <c r="T33" s="3" t="s">
@@ -12401,12 +12341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>20</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" ref="C34:P34" si="6">C6/C20</f>
+        <f t="shared" ref="C34:O34" si="6">C6/C20</f>
         <v>242.95041705282668</v>
       </c>
       <c r="D34" s="3">
@@ -12457,7 +12397,7 @@
         <v>20</v>
       </c>
       <c r="S34" s="3">
-        <f t="shared" ref="S34:AF34" si="7">S6/S20</f>
+        <f t="shared" ref="S34:AE34" si="7">S6/S20</f>
         <v>1.0885001868537973</v>
       </c>
       <c r="T34" s="3" t="s">
@@ -12502,12 +12442,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>22</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" ref="C35:P35" si="8">C7/C21</f>
+        <f t="shared" ref="C35:O35" si="8">C7/C21</f>
         <v>251.72860400912256</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -12559,7 +12499,7 @@
         <v>22</v>
       </c>
       <c r="S35" s="3">
-        <f t="shared" ref="S35:AF35" si="9">S7/S21</f>
+        <f t="shared" ref="S35:AE35" si="9">S7/S21</f>
         <v>0.9774394143056625</v>
       </c>
       <c r="T35" s="3" t="s">
@@ -12606,12 +12546,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>24</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" ref="C36:P36" si="10">C8/C22</f>
+        <f t="shared" ref="C36:O36" si="10">C8/C22</f>
         <v>266.53344136243766</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -12662,7 +12602,7 @@
         <v>24</v>
       </c>
       <c r="S36" s="3">
-        <f t="shared" ref="S36:AF36" si="11">S8/S22</f>
+        <f t="shared" ref="S36:AE36" si="11">S8/S22</f>
         <v>0.52133360512644911</v>
       </c>
       <c r="T36" s="3" t="s">
@@ -12708,12 +12648,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>26</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" ref="C37:P37" si="12">C9/C23</f>
+        <f t="shared" ref="C37:O37" si="12">C9/C23</f>
         <v>292.2452532748049</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -12758,7 +12698,6 @@
       <c r="P37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q37" s="7"/>
       <c r="R37" s="1">
         <v>26</v>
       </c>
@@ -12793,7 +12732,7 @@
         <v>0</v>
       </c>
       <c r="AC37" s="3">
-        <f t="shared" ref="S37:AF37" si="13">AC9/AC23</f>
+        <f t="shared" ref="AC37:AE37" si="13">AC9/AC23</f>
         <v>3.6719014800587507E-2</v>
       </c>
       <c r="AD37" s="3">
@@ -12807,18 +12746,13 @@
       <c r="AF37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG37" s="7"/>
-      <c r="AH37" s="7"/>
-      <c r="AI37" s="7"/>
-      <c r="AJ37" s="7"/>
-      <c r="AK37" s="7"/>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>28</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" ref="C38:P38" si="14">C10/C24</f>
+        <f t="shared" ref="C38:O38" si="14">C10/C24</f>
         <v>296.96289781577457</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -12863,7 +12797,6 @@
       <c r="P38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q38" s="7"/>
       <c r="R38" s="1">
         <v>28</v>
       </c>
@@ -12898,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="AC38" s="3">
-        <f t="shared" ref="S38:AF38" si="15">AC10/AC24</f>
+        <f t="shared" ref="AC38:AD38" si="15">AC10/AC24</f>
         <v>3.5228331780055917E-2</v>
       </c>
       <c r="AD38" s="3">
@@ -12911,18 +12844,13 @@
       <c r="AF38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG38" s="7"/>
-      <c r="AH38" s="7"/>
-      <c r="AI38" s="7"/>
-      <c r="AJ38" s="7"/>
-      <c r="AK38" s="7"/>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>30</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" ref="C39:P39" si="16">C11/C25</f>
+        <f t="shared" ref="C39:O39" si="16">C11/C25</f>
         <v>284.84811928508748</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -12967,7 +12895,6 @@
       <c r="P39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q39" s="7"/>
       <c r="R39" s="1">
         <v>30</v>
       </c>
@@ -13002,7 +12929,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="3">
-        <f t="shared" ref="S39:AF39" si="17">AC11/AC25</f>
+        <f t="shared" ref="AC39:AD39" si="17">AC11/AC25</f>
         <v>4.0401225968236275E-2</v>
       </c>
       <c r="AD39" s="3">
@@ -13015,18 +12942,13 @@
       <c r="AF39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG39" s="7"/>
-      <c r="AH39" s="7"/>
-      <c r="AI39" s="7"/>
-      <c r="AJ39" s="7"/>
-      <c r="AK39" s="7"/>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>35</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" ref="C40:P40" si="18">C12/C26</f>
+        <f t="shared" ref="C40:O40" si="18">C12/C26</f>
         <v>289.66241566131293</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -13071,7 +12993,6 @@
       <c r="P40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q40" s="7"/>
       <c r="R40" s="1">
         <v>35</v>
       </c>
@@ -13106,7 +13027,7 @@
         <v>0</v>
       </c>
       <c r="AC40" s="3">
-        <f t="shared" ref="S40:AF40" si="19">AC12/AC26</f>
+        <f t="shared" ref="AC40:AD40" si="19">AC12/AC26</f>
         <v>2.9461279461279462E-2</v>
       </c>
       <c r="AD40" s="3">
@@ -13119,13 +13040,8 @@
       <c r="AF40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="7"/>
-      <c r="AI40" s="7"/>
-      <c r="AJ40" s="7"/>
-      <c r="AK40" s="7"/>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>40</v>
       </c>
@@ -13160,7 +13076,7 @@
         <v>1</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" ref="C41:P41" si="20">M13/M27</f>
+        <f t="shared" ref="M41:O41" si="20">M13/M27</f>
         <v>13.928571428571429</v>
       </c>
       <c r="N41" s="3">
@@ -13174,7 +13090,6 @@
       <c r="P41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q41" s="7"/>
       <c r="R41" s="1">
         <v>40</v>
       </c>
@@ -13209,7 +13124,7 @@
         <v>0</v>
       </c>
       <c r="AC41" s="3">
-        <f t="shared" ref="S41:AF41" si="21">AC13/AC27</f>
+        <f t="shared" ref="AC41:AD41" si="21">AC13/AC27</f>
         <v>2.2331653687585891E-2</v>
       </c>
       <c r="AD41" s="3">
@@ -13222,13 +13137,8 @@
       <c r="AF41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="7"/>
-      <c r="AI41" s="7"/>
-      <c r="AJ41" s="7"/>
-      <c r="AK41" s="7"/>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>50</v>
       </c>
@@ -13263,7 +13173,7 @@
         <v>1</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" ref="C42:P42" si="22">M14/M28</f>
+        <f t="shared" ref="M42:O42" si="22">M14/M28</f>
         <v>7</v>
       </c>
       <c r="N42" s="3">
@@ -13277,7 +13187,6 @@
       <c r="P42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q42" s="7"/>
       <c r="R42" s="1">
         <v>50</v>
       </c>
@@ -13312,7 +13221,7 @@
         <v>0</v>
       </c>
       <c r="AC42" s="3">
-        <f t="shared" ref="S42:AF42" si="23">AC14/AC28</f>
+        <f t="shared" ref="AC42:AD42" si="23">AC14/AC28</f>
         <v>1.4665038548101327E-2</v>
       </c>
       <c r="AD42" s="3">
@@ -13325,636 +13234,37 @@
       <c r="AF42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG42" s="6"/>
-      <c r="AH42" s="7"/>
-      <c r="AI42" s="7"/>
-      <c r="AJ42" s="7"/>
-      <c r="AK42" s="7"/>
-    </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="6"/>
-      <c r="V43" s="6"/>
-      <c r="W43" s="6"/>
-      <c r="X43" s="6"/>
-      <c r="Y43" s="6"/>
-      <c r="Z43" s="6"/>
-      <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
-      <c r="AC43" s="6"/>
-      <c r="AD43" s="6"/>
-      <c r="AE43" s="6"/>
-      <c r="AF43" s="6"/>
-      <c r="AG43" s="6"/>
-      <c r="AH43" s="7"/>
-      <c r="AI43" s="7"/>
-      <c r="AJ43" s="7"/>
-      <c r="AK43" s="7"/>
-    </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
-      <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
-      <c r="W44" s="6"/>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-      <c r="AA44" s="6"/>
-      <c r="AB44" s="6"/>
-      <c r="AC44" s="6"/>
-      <c r="AD44" s="6"/>
-      <c r="AE44" s="6"/>
-      <c r="AF44" s="6"/>
-      <c r="AG44" s="6"/>
-      <c r="AH44" s="7"/>
-      <c r="AI44" s="7"/>
-      <c r="AJ44" s="7"/>
-      <c r="AK44" s="7"/>
-    </row>
-    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="6"/>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
-      <c r="AE45" s="6"/>
-      <c r="AF45" s="6"/>
-      <c r="AG45" s="6"/>
-      <c r="AH45" s="7"/>
-      <c r="AI45" s="7"/>
-      <c r="AJ45" s="7"/>
-      <c r="AK45" s="7"/>
-    </row>
-    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6"/>
-      <c r="U46" s="6"/>
-      <c r="V46" s="6"/>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6"/>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6"/>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6"/>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6"/>
-      <c r="AE46" s="6"/>
-      <c r="AF46" s="6"/>
-      <c r="AG46" s="6"/>
-      <c r="AH46" s="7"/>
-      <c r="AI46" s="7"/>
-      <c r="AJ46" s="7"/>
-      <c r="AK46" s="7"/>
-    </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P47" s="7"/>
-      <c r="Q47" s="7"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6"/>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6"/>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6"/>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6"/>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6"/>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6"/>
-      <c r="AE47" s="6"/>
-      <c r="AF47" s="6"/>
-      <c r="AG47" s="6"/>
-      <c r="AH47" s="7"/>
-      <c r="AI47" s="7"/>
-      <c r="AJ47" s="7"/>
-      <c r="AK47" s="7"/>
-    </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6"/>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6"/>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6"/>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6"/>
-      <c r="AA48" s="6"/>
-      <c r="AB48" s="6"/>
-      <c r="AC48" s="6"/>
-      <c r="AD48" s="6"/>
-      <c r="AE48" s="6"/>
-      <c r="AF48" s="6"/>
-      <c r="AG48" s="6"/>
-      <c r="AH48" s="7"/>
-      <c r="AI48" s="7"/>
-      <c r="AJ48" s="7"/>
-      <c r="AK48" s="7"/>
-    </row>
-    <row r="49" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6"/>
-      <c r="U49" s="6"/>
-      <c r="V49" s="6"/>
-      <c r="W49" s="6"/>
-      <c r="X49" s="6"/>
-      <c r="Y49" s="6"/>
-      <c r="Z49" s="6"/>
-      <c r="AA49" s="6"/>
-      <c r="AB49" s="6"/>
-      <c r="AC49" s="6"/>
-      <c r="AD49" s="6"/>
-      <c r="AE49" s="6"/>
-      <c r="AF49" s="6"/>
-      <c r="AG49" s="6"/>
-      <c r="AH49" s="7"/>
-      <c r="AI49" s="7"/>
-      <c r="AJ49" s="7"/>
-      <c r="AK49" s="7"/>
-    </row>
-    <row r="50" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="6"/>
-      <c r="T50" s="6"/>
-      <c r="U50" s="6"/>
-      <c r="V50" s="6"/>
-      <c r="W50" s="6"/>
-      <c r="X50" s="6"/>
-      <c r="Y50" s="6"/>
-      <c r="Z50" s="6"/>
-      <c r="AA50" s="6"/>
-      <c r="AB50" s="6"/>
-      <c r="AC50" s="6"/>
-      <c r="AD50" s="6"/>
-      <c r="AE50" s="6"/>
-      <c r="AF50" s="6"/>
-      <c r="AG50" s="6"/>
-      <c r="AH50" s="7"/>
-      <c r="AI50" s="7"/>
-      <c r="AJ50" s="7"/>
-      <c r="AK50" s="7"/>
-    </row>
-    <row r="51" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="6"/>
-      <c r="X51" s="6"/>
-      <c r="Y51" s="6"/>
-      <c r="Z51" s="6"/>
-      <c r="AA51" s="6"/>
-      <c r="AB51" s="6"/>
-      <c r="AC51" s="6"/>
-      <c r="AD51" s="6"/>
-      <c r="AE51" s="6"/>
-      <c r="AF51" s="6"/>
-      <c r="AG51" s="6"/>
-      <c r="AH51" s="7"/>
-      <c r="AI51" s="7"/>
-      <c r="AJ51" s="7"/>
-      <c r="AK51" s="7"/>
-    </row>
-    <row r="52" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="6"/>
-      <c r="T52" s="6"/>
-      <c r="U52" s="6"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="6"/>
-      <c r="X52" s="6"/>
-      <c r="Y52" s="6"/>
-      <c r="Z52" s="6"/>
-      <c r="AA52" s="6"/>
-      <c r="AB52" s="6"/>
-      <c r="AC52" s="6"/>
-      <c r="AD52" s="6"/>
-      <c r="AE52" s="6"/>
-      <c r="AF52" s="6"/>
-      <c r="AG52" s="6"/>
-      <c r="AH52" s="7"/>
-      <c r="AI52" s="7"/>
-      <c r="AJ52" s="7"/>
-      <c r="AK52" s="7"/>
-    </row>
-    <row r="53" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="6"/>
-      <c r="T53" s="6"/>
-      <c r="U53" s="6"/>
-      <c r="V53" s="6"/>
-      <c r="W53" s="6"/>
-      <c r="X53" s="6"/>
-      <c r="Y53" s="6"/>
-      <c r="Z53" s="6"/>
-      <c r="AA53" s="6"/>
-      <c r="AB53" s="6"/>
-      <c r="AC53" s="6"/>
-      <c r="AD53" s="6"/>
-      <c r="AE53" s="6"/>
-      <c r="AF53" s="6"/>
-      <c r="AG53" s="6"/>
-      <c r="AH53" s="7"/>
-      <c r="AI53" s="7"/>
-      <c r="AJ53" s="7"/>
-      <c r="AK53" s="7"/>
-    </row>
-    <row r="54" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6"/>
-      <c r="U54" s="6"/>
-      <c r="V54" s="6"/>
-      <c r="W54" s="6"/>
-      <c r="X54" s="6"/>
-      <c r="Y54" s="6"/>
-      <c r="Z54" s="6"/>
-      <c r="AA54" s="6"/>
-      <c r="AB54" s="6"/>
-      <c r="AC54" s="6"/>
-      <c r="AD54" s="6"/>
-      <c r="AE54" s="6"/>
-      <c r="AF54" s="6"/>
-      <c r="AG54" s="6"/>
-      <c r="AH54" s="7"/>
-      <c r="AI54" s="7"/>
-      <c r="AJ54" s="7"/>
-      <c r="AK54" s="7"/>
-    </row>
-    <row r="55" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
-      <c r="U55" s="6"/>
-      <c r="V55" s="6"/>
-      <c r="W55" s="6"/>
-      <c r="X55" s="6"/>
-      <c r="Y55" s="6"/>
-      <c r="Z55" s="6"/>
-      <c r="AA55" s="6"/>
-      <c r="AB55" s="6"/>
-      <c r="AC55" s="6"/>
-      <c r="AD55" s="6"/>
-      <c r="AE55" s="6"/>
-      <c r="AF55" s="6"/>
-      <c r="AG55" s="6"/>
-      <c r="AH55" s="7"/>
-      <c r="AI55" s="7"/>
-      <c r="AJ55" s="7"/>
-      <c r="AK55" s="7"/>
-    </row>
-    <row r="56" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="6"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="6"/>
-      <c r="U56" s="6"/>
-      <c r="V56" s="6"/>
-      <c r="W56" s="6"/>
-      <c r="X56" s="6"/>
-      <c r="Y56" s="6"/>
-      <c r="Z56" s="6"/>
-      <c r="AA56" s="6"/>
-      <c r="AB56" s="6"/>
-      <c r="AC56" s="6"/>
-      <c r="AD56" s="6"/>
-      <c r="AE56" s="6"/>
-      <c r="AF56" s="6"/>
-      <c r="AG56" s="6"/>
-      <c r="AH56" s="7"/>
-      <c r="AI56" s="7"/>
-      <c r="AJ56" s="7"/>
-      <c r="AK56" s="7"/>
-    </row>
-    <row r="57" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="6"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="6"/>
-      <c r="U57" s="6"/>
-      <c r="V57" s="6"/>
-      <c r="W57" s="6"/>
-      <c r="X57" s="6"/>
-      <c r="Y57" s="6"/>
-      <c r="Z57" s="6"/>
-      <c r="AA57" s="6"/>
-      <c r="AB57" s="6"/>
-      <c r="AC57" s="6"/>
-      <c r="AD57" s="6"/>
-      <c r="AE57" s="6"/>
-      <c r="AF57" s="6"/>
-      <c r="AG57" s="6"/>
-      <c r="AH57" s="7"/>
-      <c r="AI57" s="7"/>
-      <c r="AJ57" s="7"/>
-      <c r="AK57" s="7"/>
-    </row>
-    <row r="58" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="6"/>
-      <c r="S58" s="6"/>
-      <c r="T58" s="6"/>
-      <c r="U58" s="6"/>
-      <c r="V58" s="6"/>
-      <c r="W58" s="6"/>
-      <c r="X58" s="6"/>
-      <c r="Y58" s="6"/>
-      <c r="Z58" s="6"/>
-      <c r="AA58" s="6"/>
-      <c r="AB58" s="6"/>
-      <c r="AC58" s="6"/>
-      <c r="AD58" s="6"/>
-      <c r="AE58" s="6"/>
-      <c r="AF58" s="6"/>
-      <c r="AG58" s="6"/>
-      <c r="AH58" s="7"/>
-      <c r="AI58" s="7"/>
-      <c r="AJ58" s="7"/>
-      <c r="AK58" s="7"/>
-    </row>
-    <row r="59" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="6"/>
-      <c r="S59" s="6"/>
-      <c r="T59" s="6"/>
-      <c r="U59" s="6"/>
-      <c r="V59" s="6"/>
-      <c r="W59" s="6"/>
-      <c r="X59" s="6"/>
-      <c r="Y59" s="6"/>
-      <c r="Z59" s="6"/>
-      <c r="AA59" s="6"/>
-      <c r="AB59" s="6"/>
-      <c r="AC59" s="6"/>
-      <c r="AD59" s="6"/>
-      <c r="AE59" s="6"/>
-      <c r="AF59" s="6"/>
-      <c r="AG59" s="6"/>
-      <c r="AH59" s="7"/>
-      <c r="AI59" s="7"/>
-      <c r="AJ59" s="7"/>
-      <c r="AK59" s="7"/>
-    </row>
-    <row r="60" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="6"/>
-      <c r="S60" s="6"/>
-      <c r="T60" s="6"/>
-      <c r="U60" s="6"/>
-      <c r="V60" s="6"/>
-      <c r="W60" s="6"/>
-      <c r="X60" s="6"/>
-      <c r="Y60" s="6"/>
-      <c r="Z60" s="6"/>
-      <c r="AA60" s="6"/>
-      <c r="AB60" s="6"/>
-      <c r="AC60" s="6"/>
-      <c r="AD60" s="6"/>
-      <c r="AE60" s="6"/>
-      <c r="AF60" s="6"/>
-      <c r="AG60" s="6"/>
-      <c r="AH60" s="7"/>
-      <c r="AI60" s="7"/>
-      <c r="AJ60" s="7"/>
-      <c r="AK60" s="7"/>
-    </row>
-    <row r="61" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P61" s="7"/>
-      <c r="Q61" s="7"/>
-      <c r="R61" s="7"/>
-      <c r="S61" s="7"/>
-      <c r="T61" s="7"/>
-      <c r="U61" s="7"/>
-      <c r="V61" s="7"/>
-      <c r="W61" s="7"/>
-      <c r="X61" s="7"/>
-      <c r="Y61" s="7"/>
-      <c r="Z61" s="7"/>
-      <c r="AA61" s="7"/>
-      <c r="AB61" s="7"/>
-      <c r="AC61" s="7"/>
-      <c r="AD61" s="7"/>
-      <c r="AE61" s="7"/>
-      <c r="AF61" s="7"/>
-      <c r="AG61" s="7"/>
-      <c r="AH61" s="7"/>
-      <c r="AI61" s="7"/>
-      <c r="AJ61" s="7"/>
-      <c r="AK61" s="7"/>
-    </row>
-    <row r="62" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P62" s="7"/>
-      <c r="Q62" s="7"/>
-      <c r="R62" s="7"/>
-      <c r="S62" s="7"/>
-      <c r="T62" s="7"/>
-      <c r="U62" s="7"/>
-      <c r="V62" s="7"/>
-      <c r="W62" s="7"/>
-      <c r="X62" s="7"/>
-      <c r="Y62" s="7"/>
-      <c r="Z62" s="7"/>
-      <c r="AA62" s="7"/>
-      <c r="AB62" s="7"/>
-      <c r="AC62" s="7"/>
-      <c r="AD62" s="7"/>
-      <c r="AE62" s="7"/>
-      <c r="AF62" s="7"/>
-      <c r="AG62" s="7"/>
-      <c r="AH62" s="7"/>
-      <c r="AI62" s="7"/>
-      <c r="AJ62" s="7"/>
-      <c r="AK62" s="7"/>
-    </row>
-    <row r="63" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P63" s="7"/>
-      <c r="Q63" s="7"/>
-      <c r="R63" s="7"/>
-      <c r="S63" s="7"/>
-      <c r="T63" s="7"/>
-      <c r="U63" s="7"/>
-      <c r="V63" s="7"/>
-      <c r="W63" s="7"/>
-      <c r="X63" s="7"/>
-      <c r="Y63" s="7"/>
-      <c r="Z63" s="7"/>
-      <c r="AA63" s="7"/>
-      <c r="AB63" s="7"/>
-      <c r="AC63" s="7"/>
-      <c r="AD63" s="7"/>
-      <c r="AE63" s="7"/>
-      <c r="AF63" s="7"/>
-      <c r="AG63" s="7"/>
-      <c r="AH63" s="7"/>
-      <c r="AI63" s="7"/>
-      <c r="AJ63" s="7"/>
-      <c r="AK63" s="7"/>
-    </row>
-    <row r="64" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
-      <c r="S64" s="7"/>
-      <c r="T64" s="7"/>
-      <c r="U64" s="7"/>
-      <c r="V64" s="7"/>
-      <c r="W64" s="7"/>
-      <c r="X64" s="7"/>
-      <c r="Y64" s="7"/>
-      <c r="Z64" s="7"/>
-      <c r="AA64" s="7"/>
-      <c r="AB64" s="7"/>
-      <c r="AC64" s="7"/>
-      <c r="AD64" s="7"/>
-      <c r="AE64" s="7"/>
-      <c r="AF64" s="7"/>
-      <c r="AG64" s="7"/>
-      <c r="AH64" s="7"/>
-      <c r="AI64" s="7"/>
-      <c r="AJ64" s="7"/>
-      <c r="AK64" s="7"/>
-    </row>
-    <row r="65" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P65" s="7"/>
-      <c r="Q65" s="7"/>
-      <c r="R65" s="7"/>
-      <c r="S65" s="7"/>
-      <c r="T65" s="7"/>
-      <c r="U65" s="7"/>
-      <c r="V65" s="7"/>
-      <c r="W65" s="7"/>
-      <c r="X65" s="7"/>
-      <c r="Y65" s="7"/>
-      <c r="Z65" s="7"/>
-      <c r="AA65" s="7"/>
-      <c r="AB65" s="7"/>
-      <c r="AC65" s="7"/>
-      <c r="AD65" s="7"/>
-      <c r="AE65" s="7"/>
-      <c r="AF65" s="7"/>
-      <c r="AG65" s="7"/>
-      <c r="AH65" s="7"/>
-      <c r="AI65" s="7"/>
-      <c r="AJ65" s="7"/>
-      <c r="AK65" s="7"/>
-    </row>
-    <row r="66" spans="16:37" x14ac:dyDescent="0.25">
-      <c r="P66" s="7"/>
-      <c r="Q66" s="7"/>
-      <c r="R66" s="7"/>
-      <c r="S66" s="7"/>
-      <c r="T66" s="7"/>
-      <c r="U66" s="7"/>
-      <c r="V66" s="7"/>
-      <c r="W66" s="7"/>
-      <c r="X66" s="7"/>
-      <c r="Y66" s="7"/>
-      <c r="Z66" s="7"/>
-      <c r="AA66" s="7"/>
-      <c r="AB66" s="7"/>
-      <c r="AC66" s="7"/>
-      <c r="AD66" s="7"/>
-      <c r="AE66" s="7"/>
-      <c r="AF66" s="7"/>
-      <c r="AG66" s="7"/>
-      <c r="AH66" s="7"/>
-      <c r="AI66" s="7"/>
-      <c r="AJ66" s="7"/>
-      <c r="AK66" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:B16 O15:XFD16 A17:XFD29 A2:P14 A43:XFD1048576 A30:A42 Q30:Q42 B30 O30:P30 AG30:XFD42 R30 AE30:AF30 B31:P42 R31:AF42">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:P14 AO2:XFD14 A15:B16 O15:XFD16">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:B16 O15:XFD16 A17:XFD29 A2:P14 A43:XFD1048576 A30:A42 Q30:Q42 B30 O30:P30 AG30:XFD42 R30 AE30:AF30 B31:P42 R31:AF42">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+  <conditionalFormatting sqref="A17:XFD1048576">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:N16">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16:N16">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:N30">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:N30">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30:AD30">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30:AD30">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:AF14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:AF14">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Wrote down max k for n results.
</commit_message>
<xml_diff>
--- a/test/results/Benchmarks.xlsx
+++ b/test/results/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C10945-9266-4496-9B25-337F7E850303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF8FDCB-14C8-40AA-B8EC-001F9037E5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="22">
   <si>
     <t>CRASH</t>
   </si>
@@ -95,18 +95,39 @@
   <si>
     <t>BACK (n/k){part / us}</t>
   </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.8"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="5">
@@ -135,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,21 +179,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -226,6 +336,139 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -587,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
-  <dimension ref="B2:AP75"/>
+  <dimension ref="B2:AT75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW19" sqref="AW19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -612,9 +855,10 @@
     <col min="32" max="38" width="12" bestFit="1" customWidth="1"/>
     <col min="39" max="41" width="7" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:46">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -732,8 +976,17 @@
       <c r="AP2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="AR2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:46">
       <c r="B3" s="1">
         <v>100</v>
       </c>
@@ -851,8 +1104,17 @@
       <c r="AP3" s="3">
         <v>204226</v>
       </c>
+      <c r="AR3" s="6">
+        <v>100</v>
+      </c>
+      <c r="AS3" s="3">
+        <v>18</v>
+      </c>
+      <c r="AT3" s="3">
+        <v>11087828</v>
+      </c>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:46">
       <c r="B4" s="1">
         <v>200</v>
       </c>
@@ -970,8 +1232,17 @@
       <c r="AP4" s="3">
         <v>190569292</v>
       </c>
+      <c r="AR4" s="6">
+        <v>200</v>
+      </c>
+      <c r="AS4" s="3">
+        <v>28</v>
+      </c>
+      <c r="AT4" s="3">
+        <v>158042231843</v>
+      </c>
     </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:46">
       <c r="B5" s="1">
         <v>300</v>
       </c>
@@ -1089,8 +1360,17 @@
       <c r="AP5" s="3">
         <v>40853235313</v>
       </c>
+      <c r="AR5" s="6">
+        <v>300</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>37</v>
+      </c>
+      <c r="AT5" s="3">
+        <v>295234932551509</v>
+      </c>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:46">
       <c r="B6" s="1">
         <v>400</v>
       </c>
@@ -1208,8 +1488,17 @@
       <c r="AP6" s="3">
         <v>3972999029388</v>
       </c>
+      <c r="AR6" s="6">
+        <v>400</v>
+      </c>
+      <c r="AS6" s="3">
+        <v>45</v>
+      </c>
+      <c r="AT6" s="3">
+        <v>1.8360564956051901E+17</v>
+      </c>
     </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:46">
       <c r="B7" s="1">
         <v>500</v>
       </c>
@@ -1327,8 +1616,17 @@
       <c r="AP7" s="3">
         <v>230793554364681</v>
       </c>
+      <c r="AR7" s="6">
+        <v>500</v>
+      </c>
+      <c r="AS7" s="3">
+        <v>52</v>
+      </c>
+      <c r="AT7" s="3">
+        <v>5.5664213538686001E+19</v>
+      </c>
     </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:46">
       <c r="B8" s="1">
         <v>600</v>
       </c>
@@ -1446,8 +1744,17 @@
       <c r="AP8" s="3">
         <v>9253082936723600</v>
       </c>
+      <c r="AR8" s="6">
+        <v>600</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>58</v>
+      </c>
+      <c r="AT8" s="3">
+        <v>1.00507839698223E+22</v>
+      </c>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:46">
       <c r="B9" s="1">
         <v>700</v>
       </c>
@@ -1565,8 +1872,17 @@
       <c r="AP9" s="3">
         <v>2.7936332848370202E+17</v>
       </c>
+      <c r="AR9" s="6">
+        <v>700</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>64</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>1.2197624472627901E+24</v>
+      </c>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:46">
       <c r="B10" s="1">
         <v>800</v>
       </c>
@@ -1684,8 +2000,17 @@
       <c r="AP10" s="3">
         <v>6.7270900517410396E+18</v>
       </c>
+      <c r="AR10" s="6">
+        <v>800</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>70</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>1.0784205041118401E+26</v>
+      </c>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:46">
       <c r="B11" s="1">
         <v>900</v>
       </c>
@@ -1803,8 +2128,17 @@
       <c r="AP11" s="3">
         <v>1.34508188001572E+20</v>
       </c>
+      <c r="AR11" s="6">
+        <v>900</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>76</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>7.3441916932926802E+27</v>
+      </c>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:46">
       <c r="B12" s="1">
         <v>1000</v>
       </c>
@@ -1922,8 +2256,17 @@
       <c r="AP12" s="3">
         <v>2.3001650325743201E+21</v>
       </c>
+      <c r="AR12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>81</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>4.0177942881164098E+29</v>
+      </c>
     </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:46">
       <c r="B13" s="1">
         <v>1100</v>
       </c>
@@ -2041,8 +2384,17 @@
       <c r="AP13" s="3">
         <v>3.4403115367205001E+22</v>
       </c>
+      <c r="AR13" s="6">
+        <v>1100</v>
+      </c>
+      <c r="AS13" s="3">
+        <v>86</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>1.8208999489895201E+31</v>
+      </c>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:46">
       <c r="B14" s="1">
         <v>1200</v>
       </c>
@@ -2160,8 +2512,17 @@
       <c r="AP14" s="3">
         <v>4.5800478800814402E+23</v>
       </c>
+      <c r="AR14" s="6">
+        <v>1200</v>
+      </c>
+      <c r="AS14" s="3">
+        <v>91</v>
+      </c>
+      <c r="AT14" s="3">
+        <v>7.0072434888274296E+32</v>
+      </c>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:46">
       <c r="B15" s="1">
         <v>1300</v>
       </c>
@@ -2279,8 +2640,17 @@
       <c r="AP15" s="3">
         <v>5.5036377624997203E+24</v>
       </c>
+      <c r="AR15" s="6">
+        <v>1300</v>
+      </c>
+      <c r="AS15" s="3">
+        <v>96</v>
+      </c>
+      <c r="AT15" s="3">
+        <v>2.3348408966621102E+34</v>
+      </c>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:46">
       <c r="B16" s="1">
         <v>1400</v>
       </c>
@@ -2398,8 +2768,17 @@
       <c r="AP16" s="3">
         <v>6.0378285202834401E+25</v>
       </c>
+      <c r="AR16" s="6">
+        <v>1400</v>
+      </c>
+      <c r="AS16" s="3">
+        <v>100</v>
+      </c>
+      <c r="AT16" s="3">
+        <v>6.8463383013945207E+35</v>
+      </c>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:46">
       <c r="B17" s="1">
         <v>1500</v>
       </c>
@@ -2517,8 +2896,17 @@
       <c r="AP17" s="3">
         <v>6.1045074711796603E+26</v>
       </c>
+      <c r="AR17" s="6">
+        <v>1500</v>
+      </c>
+      <c r="AS17" s="3">
+        <v>105</v>
+      </c>
+      <c r="AT17" s="3">
+        <v>1.78963915969467E+37</v>
+      </c>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:46">
       <c r="B18" s="1">
         <v>2000</v>
       </c>
@@ -2636,8 +3024,17 @@
       <c r="AP18" s="3">
         <v>2.4061467864032602E+31</v>
       </c>
+      <c r="AR18" s="6">
+        <v>2000</v>
+      </c>
+      <c r="AS18" s="3">
+        <v>126</v>
+      </c>
+      <c r="AT18" s="3">
+        <v>5.4580732184328597E+43</v>
+      </c>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:46">
       <c r="B19" s="1">
         <v>3000</v>
       </c>
@@ -2755,8 +3152,17 @@
       <c r="AP19" s="3">
         <v>1.32946169076319E+39</v>
       </c>
+      <c r="AR19" s="6">
+        <v>3000</v>
+      </c>
+      <c r="AS19" s="3">
+        <v>162</v>
+      </c>
+      <c r="AT19" s="3">
+        <v>4.6330528909303202E+54</v>
+      </c>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:46">
       <c r="B20" s="1">
         <v>4000</v>
       </c>
@@ -2874,8 +3280,17 @@
       <c r="AP20" s="3">
         <v>4.72081917561941E+45</v>
       </c>
+      <c r="AR20" s="6">
+        <v>4000</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>194</v>
+      </c>
+      <c r="AT20" s="3">
+        <v>8.2272769426922096E+63</v>
+      </c>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:46">
       <c r="B21" s="1">
         <v>5000</v>
       </c>
@@ -2993,8 +3408,17 @@
       <c r="AP21" s="3">
         <v>2.8708755106413501E+51</v>
       </c>
+      <c r="AR21" s="6">
+        <v>5000</v>
+      </c>
+      <c r="AS21" s="3">
+        <v>223</v>
+      </c>
+      <c r="AT21" s="3">
+        <v>1.2140841128354401E+72</v>
+      </c>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:46">
       <c r="B22" s="1">
         <v>10000</v>
       </c>
@@ -3112,8 +3536,17 @@
       <c r="AP22" s="3">
         <v>1.6982016882544199E+74</v>
       </c>
+      <c r="AR22" s="6">
+        <v>10000</v>
+      </c>
+      <c r="AS22" s="3">
+        <v>341</v>
+      </c>
+      <c r="AT22" s="3">
+        <v>1.80343182120309E+104</v>
+      </c>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:46">
       <c r="B23" s="1">
         <v>20000</v>
       </c>
@@ -3225,8 +3658,17 @@
         <v>5</v>
       </c>
       <c r="AP23" s="4"/>
+      <c r="AR23" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AS23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:46">
       <c r="B24" s="1">
         <v>30000</v>
       </c>
@@ -3338,8 +3780,17 @@
         <v>5</v>
       </c>
       <c r="AP24" s="4"/>
+      <c r="AR24" s="1">
+        <v>30000</v>
+      </c>
+      <c r="AS24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT24" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:46">
       <c r="B25" s="1">
         <v>40000</v>
       </c>
@@ -3451,8 +3902,17 @@
         <v>5</v>
       </c>
       <c r="AP25" s="4"/>
+      <c r="AR25" s="1">
+        <v>40000</v>
+      </c>
+      <c r="AS25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:46">
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -3571,7 +4031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:46">
       <c r="B28" s="1">
         <v>100</v>
       </c>
@@ -3690,7 +4150,7 @@
         <v>3845884</v>
       </c>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:46">
       <c r="B29" s="1">
         <v>200</v>
       </c>
@@ -3809,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:46">
       <c r="B30" s="1">
         <v>300</v>
       </c>
@@ -3928,7 +4388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:46">
       <c r="B31" s="1">
         <v>400</v>
       </c>
@@ -4047,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:46">
       <c r="B32" s="1">
         <v>500</v>
       </c>
@@ -4166,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:42">
       <c r="B33" s="1">
         <v>600</v>
       </c>
@@ -4285,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:42">
       <c r="B34" s="1">
         <v>700</v>
       </c>
@@ -4404,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:42">
       <c r="B35" s="1">
         <v>800</v>
       </c>
@@ -4523,7 +4983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:42">
       <c r="B36" s="1">
         <v>900</v>
       </c>
@@ -4642,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:42">
       <c r="B37" s="1">
         <v>1000</v>
       </c>
@@ -4761,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:42">
       <c r="B38" s="1">
         <v>1100</v>
       </c>
@@ -4880,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:42">
       <c r="B39" s="1">
         <v>1200</v>
       </c>
@@ -4999,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:42">
       <c r="B40" s="1">
         <v>1300</v>
       </c>
@@ -5118,7 +5578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:42">
       <c r="B41" s="1">
         <v>1400</v>
       </c>
@@ -5237,7 +5697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:42">
       <c r="B42" s="1">
         <v>1500</v>
       </c>
@@ -5356,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:42">
       <c r="B43" s="1">
         <v>2000</v>
       </c>
@@ -5475,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:42">
       <c r="B44" s="1">
         <v>3000</v>
       </c>
@@ -5594,7 +6054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:42">
       <c r="B45" s="1">
         <v>4000</v>
       </c>
@@ -5713,7 +6173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:42">
       <c r="B46" s="1">
         <v>5000</v>
       </c>
@@ -5832,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:42">
       <c r="B47" s="1">
         <v>10000</v>
       </c>
@@ -5951,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:42">
       <c r="B48" s="1">
         <v>20000</v>
       </c>
@@ -6070,7 +6530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:42">
       <c r="B49" s="1">
         <v>30000</v>
       </c>
@@ -6189,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:42">
       <c r="B50" s="1">
         <v>40000</v>
       </c>
@@ -6308,7 +6768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:42">
       <c r="B52" s="1" t="s">
         <v>16</v>
       </c>
@@ -6427,7 +6887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:42">
       <c r="B53" s="1">
         <v>100</v>
       </c>
@@ -6582,7 +7042,7 @@
         <v>5.3102485670394634E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:42">
       <c r="B54" s="1">
         <v>200</v>
       </c>
@@ -6733,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:42">
       <c r="B55" s="1">
         <v>300</v>
       </c>
@@ -6881,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:42">
       <c r="B56" s="1">
         <v>400</v>
       </c>
@@ -7024,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:42">
       <c r="B57" s="1">
         <v>500</v>
       </c>
@@ -7165,7 +7625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:42">
       <c r="B58" s="1">
         <v>600</v>
       </c>
@@ -7305,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:42">
       <c r="B59" s="1">
         <v>700</v>
       </c>
@@ -7443,7 +7903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:42">
       <c r="B60" s="1">
         <v>800</v>
       </c>
@@ -7580,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:42">
       <c r="B61" s="1">
         <v>900</v>
       </c>
@@ -7717,7 +8177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:42">
       <c r="B62" s="1">
         <v>1000</v>
       </c>
@@ -7853,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:42">
       <c r="B63" s="1">
         <v>1100</v>
       </c>
@@ -7989,7 +8449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:42">
       <c r="B64" s="1">
         <v>1200</v>
       </c>
@@ -8125,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:42">
       <c r="B65" s="1">
         <v>1300</v>
       </c>
@@ -8261,7 +8721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:42">
       <c r="B66" s="1">
         <v>1400</v>
       </c>
@@ -8397,7 +8857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:42">
       <c r="B67" s="1">
         <v>1500</v>
       </c>
@@ -8531,7 +8991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:42">
       <c r="B68" s="1">
         <v>2000</v>
       </c>
@@ -8665,7 +9125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:42">
       <c r="B69" s="1">
         <v>3000</v>
       </c>
@@ -8799,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:42">
       <c r="B70" s="1">
         <v>4000</v>
       </c>
@@ -8931,7 +9391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:42">
       <c r="B71" s="1">
         <v>5000</v>
       </c>
@@ -9063,7 +9523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:42">
       <c r="B72" s="1">
         <v>10000</v>
       </c>
@@ -9190,7 +9650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:42">
       <c r="B73" s="1">
         <v>20000</v>
       </c>
@@ -9317,7 +9777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:42">
       <c r="B74" s="1">
         <v>30000</v>
       </c>
@@ -9443,7 +9903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:42">
       <c r="B75" s="1">
         <v>40000</v>
       </c>
@@ -9569,19 +10029,51 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 B2:N2 P2:AB2 AT2:XFD55 A2:A75 B3:B25 P3:P25 C25:N25 Q25:AB25 B27:AS51 AQ52:AS55 B52:AP75 AQ56:XFD75 A76:XFD1048576">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 B2:N2 P2:AB2 AT2:XFD2 A2:A75 B3:B25 P3:P25 C25:N25 Q25:AB25 B27:AS51 AQ52:AS55 B52:AP75 AQ56:XFD75 A76:XFD1048576 BA3:XFD22 AR3:AU22 AT23:XFD55">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AP2 AD3:AD25 AE25:AP25">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="AD2:AP2 AD3:AD25 AE25:AP25 AR2:AS2">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR3:AR25">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS23">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS24">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS25">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9592,13 +10084,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
-  <dimension ref="B2:AF42"/>
+  <dimension ref="B2:AK42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -9608,7 +10100,7 @@
     <col min="19" max="32" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:37">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -9699,8 +10191,17 @@
       <c r="AF2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="AH2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:37">
       <c r="B3" s="1">
         <v>14</v>
       </c>
@@ -9791,8 +10292,17 @@
       <c r="AF3" s="2">
         <v>49329280</v>
       </c>
+      <c r="AH3" s="6">
+        <v>14</v>
+      </c>
+      <c r="AI3" s="11">
+        <v>6</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>63436373</v>
+      </c>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:37">
       <c r="B4" s="1">
         <v>16</v>
       </c>
@@ -9883,8 +10393,17 @@
       <c r="AF4" s="2">
         <v>2141764053</v>
       </c>
+      <c r="AH4" s="6">
+        <v>16</v>
+      </c>
+      <c r="AI4" s="11">
+        <v>7</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>3281882604</v>
+      </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:37">
       <c r="B5" s="1">
         <v>18</v>
       </c>
@@ -9975,8 +10494,17 @@
       <c r="AF5" s="2">
         <v>106175395755</v>
       </c>
+      <c r="AH5" s="6">
+        <v>18</v>
+      </c>
+      <c r="AI5" s="11">
+        <v>7</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>197462483400</v>
+      </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:37">
       <c r="B6" s="1">
         <v>20</v>
       </c>
@@ -10067,8 +10595,17 @@
       <c r="AF6" s="2">
         <v>5917584964655</v>
       </c>
+      <c r="AH6" s="6">
+        <v>20</v>
+      </c>
+      <c r="AI6" s="11">
+        <v>8</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>15170932662679</v>
+      </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:37">
       <c r="B7" s="1">
         <v>22</v>
       </c>
@@ -10159,8 +10696,17 @@
       <c r="AF7" s="2">
         <v>366282500870286</v>
       </c>
+      <c r="AH7" s="6">
+        <v>22</v>
+      </c>
+      <c r="AI7" s="11">
+        <v>9</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>1241963303533920</v>
+      </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:37">
       <c r="B8" s="1">
         <v>24</v>
       </c>
@@ -10251,8 +10797,17 @@
       <c r="AF8" s="2">
         <v>2.49302045907582E+16</v>
       </c>
+      <c r="AH8" s="6">
+        <v>24</v>
+      </c>
+      <c r="AI8" s="11">
+        <v>9</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>1.20622574326072E+17</v>
+      </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:37">
       <c r="B9" s="1">
         <v>26</v>
       </c>
@@ -10343,8 +10898,17 @@
       <c r="AF9" s="2">
         <v>1.8505685742535501E+18</v>
       </c>
+      <c r="AH9" s="6">
+        <v>26</v>
+      </c>
+      <c r="AI9" s="11">
+        <v>10</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>1.3199555372846801E+19</v>
+      </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:37">
       <c r="B10" s="1">
         <v>28</v>
       </c>
@@ -10435,8 +10999,17 @@
       <c r="AF10" s="2">
         <v>1.4878298806437501E+20</v>
       </c>
+      <c r="AH10" s="6">
+        <v>28</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>1.53853397837477E+21</v>
+      </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:37">
       <c r="B11" s="1">
         <v>30</v>
       </c>
@@ -10527,8 +11100,17 @@
       <c r="AF11" s="2">
         <v>1.2879868072770599E+22</v>
       </c>
+      <c r="AH11" s="6">
+        <v>30</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>2.15047101560666E+23</v>
+      </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:37">
       <c r="B12" s="1">
         <v>35</v>
       </c>
@@ -10619,8 +11201,17 @@
       <c r="AF12" s="2">
         <v>2.4565469823514601E+27</v>
       </c>
+      <c r="AH12" s="6">
+        <v>35</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>12</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>6.5580126734167504E+28</v>
+      </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:37">
       <c r="B13" s="1">
         <v>40</v>
       </c>
@@ -10711,8 +11302,17 @@
       <c r="AF13" s="2">
         <v>1.62188909527975E+32</v>
       </c>
+      <c r="AH13" s="6">
+        <v>40</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>3.5859872255621798E+34</v>
+      </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:37">
       <c r="B14" s="1">
         <v>50</v>
       </c>
@@ -10803,8 +11403,24 @@
       <c r="AF14" s="2">
         <v>7.4538021532732004E+42</v>
       </c>
+      <c r="AH14" s="6">
+        <v>50</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>16</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>3.84008253654955E+46</v>
+      </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:37">
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+    </row>
+    <row r="16" spans="2:37">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -10892,11 +11508,16 @@
       <c r="AE16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AF16" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:37">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -10968,11 +11589,16 @@
       <c r="AE17" s="3">
         <v>239193</v>
       </c>
-      <c r="AF17" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:37">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -11048,11 +11674,16 @@
       <c r="AE18" s="3">
         <v>676641</v>
       </c>
-      <c r="AF18" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:37" ht="17.25">
       <c r="B19" s="1">
         <v>18</v>
       </c>
@@ -11132,11 +11763,16 @@
       <c r="AE19" s="3">
         <v>1793670</v>
       </c>
-      <c r="AF19" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:37" ht="17.25">
       <c r="B20" s="1">
         <v>20</v>
       </c>
@@ -11220,11 +11856,16 @@
       <c r="AE20" s="3">
         <v>4686700</v>
       </c>
-      <c r="AF20" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:37" ht="17.25">
       <c r="B21" s="1">
         <v>22</v>
       </c>
@@ -11312,11 +11953,16 @@
       <c r="AE21" s="3">
         <v>12414109</v>
       </c>
-      <c r="AF21" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF21" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:37" ht="17.25">
       <c r="B22" s="1">
         <v>24</v>
       </c>
@@ -11404,11 +12050,16 @@
       <c r="AE22" s="3">
         <v>41274616</v>
       </c>
-      <c r="AF22" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:37" ht="17.25">
       <c r="B23" s="1">
         <v>26</v>
       </c>
@@ -11496,11 +12147,16 @@
       <c r="AE23" s="3">
         <v>263048466</v>
       </c>
-      <c r="AF23" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="5"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:37" ht="17.25">
       <c r="B24" s="1">
         <v>28</v>
       </c>
@@ -11588,11 +12244,16 @@
       <c r="AE24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AF24" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="9"/>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:37" ht="17.25">
       <c r="B25" s="1">
         <v>30</v>
       </c>
@@ -11680,11 +12341,16 @@
       <c r="AE25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AF25" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="9"/>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:37" ht="17.25">
       <c r="B26" s="1">
         <v>35</v>
       </c>
@@ -11775,8 +12441,9 @@
       <c r="AF26" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AI26" s="5"/>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:37" ht="17.25">
       <c r="B27" s="1">
         <v>40</v>
       </c>
@@ -11867,8 +12534,9 @@
       <c r="AF27" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AI27" s="5"/>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:37" ht="17.25">
       <c r="B28" s="1">
         <v>50</v>
       </c>
@@ -11959,8 +12627,12 @@
       <c r="AF28" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AI28" s="5"/>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:37" ht="17.25">
+      <c r="AI29" s="5"/>
+    </row>
+    <row r="30" spans="2:37" ht="17.25">
       <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
@@ -12051,8 +12723,9 @@
       <c r="AF30" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="AI30" s="5"/>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:37">
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -12145,7 +12818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:37">
       <c r="B32" s="1">
         <v>16</v>
       </c>
@@ -12242,7 +12915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32">
       <c r="B33" s="1">
         <v>18</v>
       </c>
@@ -12341,7 +13014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32">
       <c r="B34" s="1">
         <v>20</v>
       </c>
@@ -12442,7 +13115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:32">
       <c r="B35" s="1">
         <v>22</v>
       </c>
@@ -12546,7 +13219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:32">
       <c r="B36" s="1">
         <v>24</v>
       </c>
@@ -12648,7 +13321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:32">
       <c r="B37" s="1">
         <v>26</v>
       </c>
@@ -12747,7 +13420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:32">
       <c r="B38" s="1">
         <v>28</v>
       </c>
@@ -12845,7 +13518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:32">
       <c r="B39" s="1">
         <v>30</v>
       </c>
@@ -12943,7 +13616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:32">
       <c r="B40" s="1">
         <v>35</v>
       </c>
@@ -13041,7 +13714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:32">
       <c r="B41" s="1">
         <v>40</v>
       </c>
@@ -13138,7 +13811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:32">
       <c r="B42" s="1">
         <v>50</v>
       </c>
@@ -13236,31 +13909,71 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:P14 AO2:XFD14 A15:B16 O15:XFD16">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:P14 AO2:XFD14 A15:B16 O15:AG16 AK15:XFD16">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:XFD1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="A31:XFD1048576 A17:AG25 AK17:XFD25 A26:AH30 AJ26:XFD30">
+    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:N16">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:AF14">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH15:AJ18 AH19:AH22 AJ19:AJ25 AH3:AH14 AJ2 AI3:AI9">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH2:AI2">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH25">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI10:AI14">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ3:AJ14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Expanded results, enabled by the improved script.
</commit_message>
<xml_diff>
--- a/test/results/Benchmarks.xlsx
+++ b/test/results/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF8FDCB-14C8-40AA-B8EC-001F9037E5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F7C4C6-E221-4A6A-A683-36752BA74D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="22">
   <si>
     <t>CRASH</t>
   </si>
@@ -196,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -210,79 +210,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -322,41 +257,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -447,14 +347,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -833,7 +733,7 @@
   <dimension ref="B2:AT75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW19" sqref="AW19"/>
+      <selection activeCell="AX21" sqref="AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3661,11 +3561,11 @@
       <c r="AR23" s="1">
         <v>20000</v>
       </c>
-      <c r="AS23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT23" s="3" t="s">
-        <v>0</v>
+      <c r="AS23" s="3">
+        <v>520</v>
+      </c>
+      <c r="AT23" s="3">
+        <v>8.7899137882931594E+149</v>
       </c>
     </row>
     <row r="24" spans="2:46">
@@ -3783,11 +3683,11 @@
       <c r="AR24" s="1">
         <v>30000</v>
       </c>
-      <c r="AS24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="3" t="s">
-        <v>0</v>
+      <c r="AS24" s="3">
+        <v>664</v>
+      </c>
+      <c r="AT24" s="3">
+        <v>1.21622887232751E+185</v>
       </c>
     </row>
     <row r="25" spans="2:46">
@@ -3905,11 +3805,11 @@
       <c r="AR25" s="1">
         <v>40000</v>
       </c>
-      <c r="AS25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT25" s="3" t="s">
-        <v>0</v>
+      <c r="AS25" s="3">
+        <v>789</v>
+      </c>
+      <c r="AT25" s="3">
+        <v>5.5715807546546397E+214</v>
       </c>
     </row>
     <row r="27" spans="2:46">
@@ -10029,51 +9929,35 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 B2:N2 P2:AB2 AT2:XFD2 A2:A75 B3:B25 P3:P25 C25:N25 Q25:AB25 B27:AS51 AQ52:AS55 B52:AP75 AQ56:XFD75 A76:XFD1048576 BA3:XFD22 AR3:AU22 AT23:XFD55">
-    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 B2:N2 P2:AB2 A2:A75 AR3:AU22 BA3:XFD22 B3:B25 P3:P25 AT23:XFD55 C25:N25 Q25:AB25 B27:AS51 AQ52:AS55 B52:AP75 AQ56:XFD75 A76:XFD1048576">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AP2 AD3:AD25 AE25:AP25 AR2:AS2">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
+  <conditionalFormatting sqref="AD2:AP2 AR2:XFD2 AD3:AD25 AE25:AP25">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR3:AR25">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS23">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+  <conditionalFormatting sqref="AS23:AS25">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS24">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS25">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10084,7 +9968,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
-  <dimension ref="B2:AK42"/>
+  <dimension ref="B2:AJ42"/>
   <sheetViews>
     <sheetView topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AK8" sqref="AK8"/>
@@ -10100,7 +9984,7 @@
     <col min="19" max="32" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:37">
+    <row r="2" spans="2:36">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -10201,7 +10085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:37">
+    <row r="3" spans="2:36">
       <c r="B3" s="1">
         <v>14</v>
       </c>
@@ -10295,14 +10179,14 @@
       <c r="AH3" s="6">
         <v>14</v>
       </c>
-      <c r="AI3" s="11">
+      <c r="AI3" s="3">
         <v>6</v>
       </c>
       <c r="AJ3" s="3">
         <v>63436373</v>
       </c>
     </row>
-    <row r="4" spans="2:37">
+    <row r="4" spans="2:36">
       <c r="B4" s="1">
         <v>16</v>
       </c>
@@ -10396,14 +10280,14 @@
       <c r="AH4" s="6">
         <v>16</v>
       </c>
-      <c r="AI4" s="11">
+      <c r="AI4" s="3">
         <v>7</v>
       </c>
       <c r="AJ4" s="3">
         <v>3281882604</v>
       </c>
     </row>
-    <row r="5" spans="2:37">
+    <row r="5" spans="2:36">
       <c r="B5" s="1">
         <v>18</v>
       </c>
@@ -10497,14 +10381,14 @@
       <c r="AH5" s="6">
         <v>18</v>
       </c>
-      <c r="AI5" s="11">
+      <c r="AI5" s="3">
         <v>7</v>
       </c>
       <c r="AJ5" s="3">
         <v>197462483400</v>
       </c>
     </row>
-    <row r="6" spans="2:37">
+    <row r="6" spans="2:36">
       <c r="B6" s="1">
         <v>20</v>
       </c>
@@ -10598,14 +10482,14 @@
       <c r="AH6" s="6">
         <v>20</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6" s="3">
         <v>8</v>
       </c>
       <c r="AJ6" s="3">
         <v>15170932662679</v>
       </c>
     </row>
-    <row r="7" spans="2:37">
+    <row r="7" spans="2:36">
       <c r="B7" s="1">
         <v>22</v>
       </c>
@@ -10699,14 +10583,14 @@
       <c r="AH7" s="6">
         <v>22</v>
       </c>
-      <c r="AI7" s="11">
+      <c r="AI7" s="3">
         <v>9</v>
       </c>
       <c r="AJ7" s="3">
         <v>1241963303533920</v>
       </c>
     </row>
-    <row r="8" spans="2:37">
+    <row r="8" spans="2:36">
       <c r="B8" s="1">
         <v>24</v>
       </c>
@@ -10800,14 +10684,14 @@
       <c r="AH8" s="6">
         <v>24</v>
       </c>
-      <c r="AI8" s="11">
+      <c r="AI8" s="3">
         <v>9</v>
       </c>
       <c r="AJ8" s="3">
         <v>1.20622574326072E+17</v>
       </c>
     </row>
-    <row r="9" spans="2:37">
+    <row r="9" spans="2:36">
       <c r="B9" s="1">
         <v>26</v>
       </c>
@@ -10901,14 +10785,14 @@
       <c r="AH9" s="6">
         <v>26</v>
       </c>
-      <c r="AI9" s="11">
+      <c r="AI9" s="3">
         <v>10</v>
       </c>
       <c r="AJ9" s="3">
         <v>1.3199555372846801E+19</v>
       </c>
     </row>
-    <row r="10" spans="2:37">
+    <row r="10" spans="2:36">
       <c r="B10" s="1">
         <v>28</v>
       </c>
@@ -11009,7 +10893,7 @@
         <v>1.53853397837477E+21</v>
       </c>
     </row>
-    <row r="11" spans="2:37">
+    <row r="11" spans="2:36">
       <c r="B11" s="1">
         <v>30</v>
       </c>
@@ -11110,7 +10994,7 @@
         <v>2.15047101560666E+23</v>
       </c>
     </row>
-    <row r="12" spans="2:37">
+    <row r="12" spans="2:36">
       <c r="B12" s="1">
         <v>35</v>
       </c>
@@ -11211,7 +11095,7 @@
         <v>6.5580126734167504E+28</v>
       </c>
     </row>
-    <row r="13" spans="2:37">
+    <row r="13" spans="2:36">
       <c r="B13" s="1">
         <v>40</v>
       </c>
@@ -11312,7 +11196,7 @@
         <v>3.5859872255621798E+34</v>
       </c>
     </row>
-    <row r="14" spans="2:37">
+    <row r="14" spans="2:36">
       <c r="B14" s="1">
         <v>50</v>
       </c>
@@ -11413,14 +11297,10 @@
         <v>3.84008253654955E+46</v>
       </c>
     </row>
-    <row r="15" spans="2:37">
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
+    <row r="15" spans="2:36">
+      <c r="AH15" s="9"/>
     </row>
-    <row r="16" spans="2:37">
+    <row r="16" spans="2:36">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -11511,13 +11391,9 @@
       <c r="AF16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
+      <c r="AH16" s="9"/>
     </row>
-    <row r="17" spans="2:37">
+    <row r="17" spans="2:35">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -11592,13 +11468,9 @@
       <c r="AF17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
+      <c r="AH17" s="9"/>
     </row>
-    <row r="18" spans="2:37">
+    <row r="18" spans="2:35">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -11677,13 +11549,9 @@
       <c r="AF18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="9"/>
-      <c r="AJ18" s="9"/>
-      <c r="AK18" s="9"/>
+      <c r="AH18" s="9"/>
     </row>
-    <row r="19" spans="2:37" ht="17.25">
+    <row r="19" spans="2:35" ht="17.25">
       <c r="B19" s="1">
         <v>18</v>
       </c>
@@ -11766,13 +11634,10 @@
       <c r="AF19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="10"/>
+      <c r="AH19" s="9"/>
       <c r="AI19" s="5"/>
-      <c r="AJ19" s="9"/>
-      <c r="AK19" s="9"/>
     </row>
-    <row r="20" spans="2:37" ht="17.25">
+    <row r="20" spans="2:35" ht="17.25">
       <c r="B20" s="1">
         <v>20</v>
       </c>
@@ -11859,13 +11724,10 @@
       <c r="AF20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="10"/>
+      <c r="AH20" s="9"/>
       <c r="AI20" s="5"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
     </row>
-    <row r="21" spans="2:37" ht="17.25">
+    <row r="21" spans="2:35" ht="17.25">
       <c r="B21" s="1">
         <v>22</v>
       </c>
@@ -11956,13 +11818,10 @@
       <c r="AF21" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="10"/>
+      <c r="AH21" s="9"/>
       <c r="AI21" s="5"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
     </row>
-    <row r="22" spans="2:37" ht="17.25">
+    <row r="22" spans="2:35" ht="17.25">
       <c r="B22" s="1">
         <v>24</v>
       </c>
@@ -12053,13 +11912,10 @@
       <c r="AF22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="10"/>
+      <c r="AH22" s="9"/>
       <c r="AI22" s="5"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
     </row>
-    <row r="23" spans="2:37" ht="17.25">
+    <row r="23" spans="2:35" ht="17.25">
       <c r="B23" s="1">
         <v>26</v>
       </c>
@@ -12150,13 +12006,9 @@
       <c r="AF23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
       <c r="AI23" s="5"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
     </row>
-    <row r="24" spans="2:37" ht="17.25">
+    <row r="24" spans="2:35" ht="17.25">
       <c r="B24" s="1">
         <v>28</v>
       </c>
@@ -12247,13 +12099,9 @@
       <c r="AF24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
       <c r="AI24" s="5"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
     </row>
-    <row r="25" spans="2:37" ht="17.25">
+    <row r="25" spans="2:35" ht="17.25">
       <c r="B25" s="1">
         <v>30</v>
       </c>
@@ -12344,13 +12192,9 @@
       <c r="AF25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
       <c r="AI25" s="5"/>
-      <c r="AJ25" s="9"/>
-      <c r="AK25" s="9"/>
     </row>
-    <row r="26" spans="2:37" ht="17.25">
+    <row r="26" spans="2:35" ht="17.25">
       <c r="B26" s="1">
         <v>35</v>
       </c>
@@ -12443,7 +12287,7 @@
       </c>
       <c r="AI26" s="5"/>
     </row>
-    <row r="27" spans="2:37" ht="17.25">
+    <row r="27" spans="2:35" ht="17.25">
       <c r="B27" s="1">
         <v>40</v>
       </c>
@@ -12536,7 +12380,7 @@
       </c>
       <c r="AI27" s="5"/>
     </row>
-    <row r="28" spans="2:37" ht="17.25">
+    <row r="28" spans="2:35" ht="17.25">
       <c r="B28" s="1">
         <v>50</v>
       </c>
@@ -12629,10 +12473,10 @@
       </c>
       <c r="AI28" s="5"/>
     </row>
-    <row r="29" spans="2:37" ht="17.25">
+    <row r="29" spans="2:35" ht="17.25">
       <c r="AI29" s="5"/>
     </row>
-    <row r="30" spans="2:37" ht="17.25">
+    <row r="30" spans="2:35" ht="17.25">
       <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
@@ -12725,7 +12569,7 @@
       </c>
       <c r="AI30" s="5"/>
     </row>
-    <row r="31" spans="2:37">
+    <row r="31" spans="2:35">
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -12818,7 +12662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:37">
+    <row r="32" spans="2:35">
       <c r="B32" s="1">
         <v>16</v>
       </c>
@@ -13909,75 +13753,75 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:P14 AO2:XFD14 A15:B16 O15:AG16 AK15:XFD16">
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:P14 AO2:XFD14 A15:B16 O15:AG16">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:XFD1048576 A17:AG25 AK17:XFD25 A26:AH30 AJ26:XFD30">
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:N16">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:AF14">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH15:AJ18 AH19:AH22 AJ19:AJ25 AH3:AH14 AJ2 AI3:AI9">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+  <conditionalFormatting sqref="AH3:AH25">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AI2">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH25">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+  <conditionalFormatting sqref="AH15:AJ18 AJ19:AJ25">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10:AI14">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+  <conditionalFormatting sqref="AI3:AI14">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3:AJ14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="AJ2:AJ14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK15:XFD25 A17:AG25 A26:AH30 AJ26:XFD30 A31:XFD1048576">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added plots to results.
</commit_message>
<xml_diff>
--- a/test/results/Benchmarks.xlsx
+++ b/test/results/Benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F7C4C6-E221-4A6A-A683-36752BA74D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF51F04-D325-4E82-A693-899BEA81727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -413,6 +413,1995 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Најзаступљенији број делова (цели бројеви)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Најзаступљенији број делова</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Integer Partitioning'!$AR$3:$AR$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Integer Partitioning'!$AS$3:$AS$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>789</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-B062-4AB2-933C-993EB545EAAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1233452896"/>
+        <c:axId val="1233440416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1233452896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233440416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1233440416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1233452896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Најзаступљенији број делова (скупови)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Set Partitioning'!$AH$3:$AH$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Set Partitioning'!$AI$3:$AI$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A2AE-45A1-861A-17F488DB834A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2012403696"/>
+        <c:axId val="2012285952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2012403696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2012285952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2012285952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2012403696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97D49C7C-497A-6968-AC3D-17B0920ECE39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>2264</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12348</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>290648</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127702</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F9EE632-DD4B-5826-FC99-512FB69F9786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -733,7 +2722,7 @@
   <dimension ref="B2:AT75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX21" sqref="AX21"/>
+      <selection activeCell="AV26" sqref="AV26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9963,6 +11952,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9970,8 +11960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
   <dimension ref="B2:AJ42"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN25" sqref="AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13826,5 +15816,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more plots to results.
</commit_message>
<xml_diff>
--- a/test/results/Benchmarks.xlsx
+++ b/test/results/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF51F04-D325-4E82-A693-899BEA81727D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B64F81-E457-445E-A3DC-EDAB4DDDE0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Integer Partitioning" sheetId="1" r:id="rId1"/>
@@ -871,6 +871,450 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Број партиција с најзаступљенијим бројем делова</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Број партиција с највећим бројем делова</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Integer Partitioning'!$AR$3:$AR$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Integer Partitioning'!$AT$3:$AT$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>11087828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158042231843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>295234932551509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8360564956051901E+17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5664213538686001E+19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.00507839698223E+22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2197624472627901E+24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0784205041118401E+26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3441916932926802E+27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0177942881164098E+29</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8208999489895201E+31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0072434888274296E+32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3348408966621102E+34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8463383013945207E+35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.78963915969467E+37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4580732184328597E+43</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.6330528909303202E+54</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.2272769426922096E+63</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2140841128354401E+72</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.80343182120309E+104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.7899137882931594E+149</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.21622887232751E+185</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.5715807546546397E+214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-56AB-4F99-81D2-5D7DB9EB62E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="672889824"/>
+        <c:axId val="672890304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="672889824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672890304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="672890304"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672889824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1208,6 +1652,359 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Број партиција са најзаступљенијим бројем делова</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Set Partitioning'!$AH$3:$AH$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Set Partitioning'!$AJ$3:$AJ$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>63436373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3281882604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197462483400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15170932662679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1241963303533920</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.20622574326072E+17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3199555372846801E+19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.53853397837477E+21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.15047101560666E+23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5580126734167504E+28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5859872255621798E+34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.84008253654955E+46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E9FA-4BBE-A0D2-DD2A0D135C80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="965077728"/>
+        <c:axId val="965054208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="965077728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="965054208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="965054208"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="965077728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1249,6 +2046,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2320,6 +3197,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2353,6 +4262,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>5602</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>12326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>341778</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69342CC-8E68-D621-4CA0-A5B63F23CD4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2394,6 +4339,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F2A1FBE-4477-3125-C1A7-E879E5905E63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2721,8 +4702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AT75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV26" sqref="AV26"/>
+    <sheetView topLeftCell="W5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT34" sqref="AT34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11960,8 +13941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
   <dimension ref="B2:AJ42"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN25" sqref="AN25"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ30" sqref="AJ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>